<commit_message>
Add fetch file to autorun scripts to generate new plots each day.
</commit_message>
<xml_diff>
--- a/Harris_Data.xlsx
+++ b/Harris_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>06-08-2020</t>
+  </si>
+  <si>
+    <t>06-09-2020</t>
   </si>
 </sst>
 </file>
@@ -584,7 +587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1927,6 +1930,26 @@
         <v>14656</v>
       </c>
     </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>71</v>
+      </c>
+      <c r="C68">
+        <v>15238</v>
+      </c>
+      <c r="D68">
+        <v>262</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>14976</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Found missing Harris Co. data.
</commit_message>
<xml_diff>
--- a/Harris_Data.xlsx
+++ b/Harris_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>Date</t>
   </si>
@@ -53,6 +53,45 @@
   </si>
   <si>
     <t>03-29-2020</t>
+  </si>
+  <si>
+    <t>03-30-2020</t>
+  </si>
+  <si>
+    <t>03-31-2020</t>
+  </si>
+  <si>
+    <t>04-01-2020</t>
+  </si>
+  <si>
+    <t>04-02-2020</t>
+  </si>
+  <si>
+    <t>04-03-2020</t>
+  </si>
+  <si>
+    <t>04-04-2020</t>
+  </si>
+  <si>
+    <t>04-05-2020</t>
+  </si>
+  <si>
+    <t>04-06-2020</t>
+  </si>
+  <si>
+    <t>04-07-2020</t>
+  </si>
+  <si>
+    <t>04-08-2020</t>
+  </si>
+  <si>
+    <t>04-09-2020</t>
+  </si>
+  <si>
+    <t>04-10-2020</t>
+  </si>
+  <si>
+    <t>04-11-2020</t>
   </si>
   <si>
     <t>04-12-2020</t>
@@ -587,7 +626,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -778,16 +817,16 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>3629</v>
+        <v>563</v>
       </c>
       <c r="D10">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>3585</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -798,16 +837,16 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>3744</v>
+        <v>680</v>
       </c>
       <c r="D11">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>3698</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -818,16 +857,16 @@
         <v>15</v>
       </c>
       <c r="C12">
-        <v>3907</v>
+        <v>847</v>
       </c>
       <c r="D12">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>3855</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -838,16 +877,16 @@
         <v>16</v>
       </c>
       <c r="C13">
-        <v>4097</v>
+        <v>955</v>
       </c>
       <c r="D13">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>4039</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -858,16 +897,16 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>4306</v>
+        <v>1106</v>
       </c>
       <c r="D14">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>4243</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -878,16 +917,16 @@
         <v>18</v>
       </c>
       <c r="C15">
-        <v>4460</v>
+        <v>1284</v>
       </c>
       <c r="D15">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>4393</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -898,16 +937,16 @@
         <v>19</v>
       </c>
       <c r="C16">
-        <v>4653</v>
+        <v>1395</v>
       </c>
       <c r="D16">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>4582</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -918,16 +957,16 @@
         <v>20</v>
       </c>
       <c r="C17">
-        <v>4823</v>
+        <v>1809</v>
       </c>
       <c r="D17">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>4748</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -938,16 +977,16 @@
         <v>21</v>
       </c>
       <c r="C18">
-        <v>4977</v>
+        <v>2146</v>
       </c>
       <c r="D18">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>4899</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -958,16 +997,16 @@
         <v>22</v>
       </c>
       <c r="C19">
-        <v>5143</v>
+        <v>2341</v>
       </c>
       <c r="D19">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>5064</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -978,16 +1017,16 @@
         <v>23</v>
       </c>
       <c r="C20">
-        <v>5211</v>
+        <v>3047</v>
       </c>
       <c r="D20">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>5131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -998,16 +1037,16 @@
         <v>24</v>
       </c>
       <c r="C21">
-        <v>5330</v>
+        <v>3261</v>
       </c>
       <c r="D21">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>5248</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1018,16 +1057,16 @@
         <v>25</v>
       </c>
       <c r="C22">
-        <v>5482</v>
+        <v>3561</v>
       </c>
       <c r="D22">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
-        <v>5398</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1038,16 +1077,16 @@
         <v>26</v>
       </c>
       <c r="C23">
-        <v>5482</v>
+        <v>3629</v>
       </c>
       <c r="D23">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>5398</v>
+        <v>3585</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1058,16 +1097,16 @@
         <v>27</v>
       </c>
       <c r="C24">
-        <v>5628</v>
+        <v>3744</v>
       </c>
       <c r="D24">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <v>5544</v>
+        <v>3698</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1078,16 +1117,16 @@
         <v>28</v>
       </c>
       <c r="C25">
-        <v>5628</v>
+        <v>3907</v>
       </c>
       <c r="D25">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>5544</v>
+        <v>3855</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1098,16 +1137,16 @@
         <v>29</v>
       </c>
       <c r="C26">
-        <v>5827</v>
+        <v>4097</v>
       </c>
       <c r="D26">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>5729</v>
+        <v>4039</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1118,16 +1157,16 @@
         <v>30</v>
       </c>
       <c r="C27">
-        <v>6161</v>
+        <v>4306</v>
       </c>
       <c r="D27">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>6052</v>
+        <v>4243</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1138,16 +1177,16 @@
         <v>31</v>
       </c>
       <c r="C28">
-        <v>6356</v>
+        <v>4460</v>
       </c>
       <c r="D28">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>6242</v>
+        <v>4393</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1158,16 +1197,16 @@
         <v>32</v>
       </c>
       <c r="C29">
-        <v>6551</v>
+        <v>4653</v>
       </c>
       <c r="D29">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>6429</v>
+        <v>4582</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1178,16 +1217,16 @@
         <v>33</v>
       </c>
       <c r="C30">
-        <v>6708</v>
+        <v>4823</v>
       </c>
       <c r="D30">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>6579</v>
+        <v>4748</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1198,16 +1237,16 @@
         <v>34</v>
       </c>
       <c r="C31">
-        <v>6838</v>
+        <v>4977</v>
       </c>
       <c r="D31">
-        <v>133</v>
+        <v>78</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>6705</v>
+        <v>4899</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1218,16 +1257,16 @@
         <v>35</v>
       </c>
       <c r="C32">
-        <v>6967</v>
+        <v>5143</v>
       </c>
       <c r="D32">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>6827</v>
+        <v>5064</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1238,16 +1277,16 @@
         <v>36</v>
       </c>
       <c r="C33">
-        <v>7128</v>
+        <v>5211</v>
       </c>
       <c r="D33">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>6984</v>
+        <v>5131</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1258,16 +1297,16 @@
         <v>37</v>
       </c>
       <c r="C34">
-        <v>7244</v>
+        <v>5330</v>
       </c>
       <c r="D34">
-        <v>150</v>
+        <v>82</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>7094</v>
+        <v>5248</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1278,16 +1317,16 @@
         <v>38</v>
       </c>
       <c r="C35">
-        <v>7377</v>
+        <v>5482</v>
       </c>
       <c r="D35">
-        <v>154</v>
+        <v>84</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
-        <v>7223</v>
+        <v>5398</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1298,16 +1337,16 @@
         <v>39</v>
       </c>
       <c r="C36">
-        <v>7594</v>
+        <v>5482</v>
       </c>
       <c r="D36">
-        <v>160</v>
+        <v>84</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>7434</v>
+        <v>5398</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1318,16 +1357,16 @@
         <v>40</v>
       </c>
       <c r="C37">
-        <v>7803</v>
+        <v>5628</v>
       </c>
       <c r="D37">
-        <v>168</v>
+        <v>84</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <v>7635</v>
+        <v>5544</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1338,16 +1377,16 @@
         <v>41</v>
       </c>
       <c r="C38">
-        <v>7878</v>
+        <v>5628</v>
       </c>
       <c r="D38">
-        <v>172</v>
+        <v>84</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>7706</v>
+        <v>5544</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1358,16 +1397,16 @@
         <v>42</v>
       </c>
       <c r="C39">
-        <v>8176</v>
+        <v>5827</v>
       </c>
       <c r="D39">
-        <v>179</v>
+        <v>98</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>7997</v>
+        <v>5729</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1378,16 +1417,16 @@
         <v>43</v>
       </c>
       <c r="C40">
-        <v>8416</v>
+        <v>6161</v>
       </c>
       <c r="D40">
-        <v>183</v>
+        <v>109</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>8233</v>
+        <v>6052</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1398,16 +1437,16 @@
         <v>44</v>
       </c>
       <c r="C41">
-        <v>8621</v>
+        <v>6356</v>
       </c>
       <c r="D41">
-        <v>188</v>
+        <v>114</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>8433</v>
+        <v>6242</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1418,16 +1457,16 @@
         <v>45</v>
       </c>
       <c r="C42">
-        <v>8817</v>
+        <v>6551</v>
       </c>
       <c r="D42">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>8624</v>
+        <v>6429</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1438,16 +1477,16 @@
         <v>46</v>
       </c>
       <c r="C43">
-        <v>9050</v>
+        <v>6708</v>
       </c>
       <c r="D43">
-        <v>193</v>
+        <v>129</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43">
-        <v>8857</v>
+        <v>6579</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1458,16 +1497,16 @@
         <v>47</v>
       </c>
       <c r="C44">
-        <v>9126</v>
+        <v>6838</v>
       </c>
       <c r="D44">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44">
-        <v>8922</v>
+        <v>6705</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1478,16 +1517,16 @@
         <v>48</v>
       </c>
       <c r="C45">
-        <v>9465</v>
+        <v>6967</v>
       </c>
       <c r="D45">
-        <v>204</v>
+        <v>140</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45">
-        <v>9261</v>
+        <v>6827</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1498,16 +1537,16 @@
         <v>49</v>
       </c>
       <c r="C46">
-        <v>9635</v>
+        <v>7128</v>
       </c>
       <c r="D46">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46">
-        <v>9430</v>
+        <v>6984</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1518,16 +1557,16 @@
         <v>50</v>
       </c>
       <c r="C47">
-        <v>9859</v>
+        <v>7244</v>
       </c>
       <c r="D47">
-        <v>207</v>
+        <v>150</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
-        <v>9652</v>
+        <v>7094</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1538,16 +1577,16 @@
         <v>51</v>
       </c>
       <c r="C48">
-        <v>10095</v>
+        <v>7377</v>
       </c>
       <c r="D48">
-        <v>210</v>
+        <v>154</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>9885</v>
+        <v>7223</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1558,16 +1597,16 @@
         <v>52</v>
       </c>
       <c r="C49">
-        <v>10283</v>
+        <v>7594</v>
       </c>
       <c r="D49">
-        <v>216</v>
+        <v>160</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <v>10067</v>
+        <v>7434</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1578,16 +1617,16 @@
         <v>53</v>
       </c>
       <c r="C50">
-        <v>10526</v>
+        <v>7803</v>
       </c>
       <c r="D50">
-        <v>217</v>
+        <v>168</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <v>10309</v>
+        <v>7635</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1598,16 +1637,16 @@
         <v>54</v>
       </c>
       <c r="C51">
-        <v>10770</v>
+        <v>7878</v>
       </c>
       <c r="D51">
-        <v>219</v>
+        <v>172</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="F51">
-        <v>10551</v>
+        <v>7706</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1618,16 +1657,16 @@
         <v>55</v>
       </c>
       <c r="C52">
-        <v>10921</v>
+        <v>8176</v>
       </c>
       <c r="D52">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <v>10701</v>
+        <v>7997</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1638,16 +1677,16 @@
         <v>56</v>
       </c>
       <c r="C53">
-        <v>10995</v>
+        <v>8416</v>
       </c>
       <c r="D53">
-        <v>221</v>
+        <v>183</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="F53">
-        <v>10774</v>
+        <v>8233</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1658,16 +1697,16 @@
         <v>57</v>
       </c>
       <c r="C54">
-        <v>11281</v>
+        <v>8621</v>
       </c>
       <c r="D54">
-        <v>221</v>
+        <v>188</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54">
-        <v>11060</v>
+        <v>8433</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1678,16 +1717,16 @@
         <v>58</v>
       </c>
       <c r="C55">
-        <v>11542</v>
+        <v>8817</v>
       </c>
       <c r="D55">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="F55">
-        <v>11319</v>
+        <v>8624</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1698,16 +1737,16 @@
         <v>59</v>
       </c>
       <c r="C56">
-        <v>11770</v>
+        <v>9050</v>
       </c>
       <c r="D56">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="E56">
         <v>0</v>
       </c>
       <c r="F56">
-        <v>11546</v>
+        <v>8857</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1718,16 +1757,16 @@
         <v>60</v>
       </c>
       <c r="C57">
-        <v>12009</v>
+        <v>9126</v>
       </c>
       <c r="D57">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="F57">
-        <v>11781</v>
+        <v>8922</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1738,16 +1777,16 @@
         <v>61</v>
       </c>
       <c r="C58">
-        <v>12220</v>
+        <v>9465</v>
       </c>
       <c r="D58">
-        <v>231</v>
+        <v>204</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
-        <v>11989</v>
+        <v>9261</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1758,16 +1797,16 @@
         <v>62</v>
       </c>
       <c r="C59">
-        <v>12276</v>
+        <v>9635</v>
       </c>
       <c r="D59">
-        <v>232</v>
+        <v>205</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
       <c r="F59">
-        <v>12044</v>
+        <v>9430</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1778,16 +1817,16 @@
         <v>63</v>
       </c>
       <c r="C60">
-        <v>12664</v>
+        <v>9859</v>
       </c>
       <c r="D60">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60">
-        <v>12429</v>
+        <v>9652</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1798,16 +1837,16 @@
         <v>64</v>
       </c>
       <c r="C61">
-        <v>13027</v>
+        <v>10095</v>
       </c>
       <c r="D61">
-        <v>236</v>
+        <v>210</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61">
-        <v>12791</v>
+        <v>9885</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1818,16 +1857,16 @@
         <v>65</v>
       </c>
       <c r="C62">
-        <v>13268</v>
+        <v>10283</v>
       </c>
       <c r="D62">
-        <v>241</v>
+        <v>216</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
       <c r="F62">
-        <v>13027</v>
+        <v>10067</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1838,16 +1877,16 @@
         <v>66</v>
       </c>
       <c r="C63">
-        <v>13603</v>
+        <v>10526</v>
       </c>
       <c r="D63">
-        <v>247</v>
+        <v>217</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63">
-        <v>13356</v>
+        <v>10309</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1858,16 +1897,16 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>13940</v>
+        <v>10770</v>
       </c>
       <c r="D64">
-        <v>253</v>
+        <v>219</v>
       </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64">
-        <v>13687</v>
+        <v>10551</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1878,16 +1917,16 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>14423</v>
+        <v>10921</v>
       </c>
       <c r="D65">
-        <v>259</v>
+        <v>220</v>
       </c>
       <c r="E65">
         <v>0</v>
       </c>
       <c r="F65">
-        <v>14164</v>
+        <v>10701</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1898,16 +1937,16 @@
         <v>69</v>
       </c>
       <c r="C66">
-        <v>14586</v>
+        <v>10995</v>
       </c>
       <c r="D66">
-        <v>261</v>
+        <v>221</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66">
-        <v>14325</v>
+        <v>10774</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1918,16 +1957,16 @@
         <v>70</v>
       </c>
       <c r="C67">
-        <v>14918</v>
+        <v>11281</v>
       </c>
       <c r="D67">
-        <v>262</v>
+        <v>221</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="F67">
-        <v>14656</v>
+        <v>11060</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1938,15 +1977,275 @@
         <v>71</v>
       </c>
       <c r="C68">
+        <v>11542</v>
+      </c>
+      <c r="D68">
+        <v>223</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>11319</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69">
+        <v>11770</v>
+      </c>
+      <c r="D69">
+        <v>224</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>11546</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70">
+        <v>12009</v>
+      </c>
+      <c r="D70">
+        <v>228</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>11781</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>74</v>
+      </c>
+      <c r="C71">
+        <v>12220</v>
+      </c>
+      <c r="D71">
+        <v>231</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>11989</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72">
+        <v>12276</v>
+      </c>
+      <c r="D72">
+        <v>232</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>12044</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73">
+        <v>12664</v>
+      </c>
+      <c r="D73">
+        <v>235</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>12429</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74">
+        <v>13027</v>
+      </c>
+      <c r="D74">
+        <v>236</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>12791</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>78</v>
+      </c>
+      <c r="C75">
+        <v>13268</v>
+      </c>
+      <c r="D75">
+        <v>241</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>13027</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76">
+        <v>13603</v>
+      </c>
+      <c r="D76">
+        <v>247</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>13356</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77">
+        <v>13940</v>
+      </c>
+      <c r="D77">
+        <v>253</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>13687</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78">
+        <v>14423</v>
+      </c>
+      <c r="D78">
+        <v>259</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>14164</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79">
+        <v>14586</v>
+      </c>
+      <c r="D79">
+        <v>261</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>14325</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80">
+        <v>14918</v>
+      </c>
+      <c r="D80">
+        <v>262</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>14656</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81">
         <v>15238</v>
       </c>
-      <c r="D68">
+      <c r="D81">
         <v>262</v>
       </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68">
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
         <v>14976</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test digital ocean commit
</commit_message>
<xml_diff>
--- a/Harris_Data.xlsx
+++ b/Harris_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
   </si>
   <si>
     <t>Date</t>
@@ -677,13 +686,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T84"/>
+  <dimension ref="A1:W84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:23">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,8 +750,17 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -788,23 +806,32 @@
       <c r="O2">
         <v>0</v>
       </c>
-      <c r="P2" t="s">
-        <v>19</v>
+      <c r="P2">
+        <v>0</v>
       </c>
       <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2">
         <v>74</v>
       </c>
-      <c r="R2">
+      <c r="U2">
         <v>1</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -850,23 +877,32 @@
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
-        <v>20</v>
+      <c r="P3">
+        <v>1</v>
       </c>
       <c r="Q3">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="R3">
         <v>1</v>
       </c>
-      <c r="S3">
-        <v>0</v>
+      <c r="S3" t="s">
+        <v>23</v>
       </c>
       <c r="T3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+        <v>78</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -912,23 +948,32 @@
       <c r="O4">
         <v>2</v>
       </c>
-      <c r="P4" t="s">
-        <v>21</v>
+      <c r="P4">
+        <v>2</v>
       </c>
       <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="S4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4">
         <v>134</v>
       </c>
-      <c r="R4">
+      <c r="U4">
         <v>1</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -974,23 +1019,32 @@
       <c r="O5">
         <v>3</v>
       </c>
-      <c r="P5" t="s">
-        <v>22</v>
+      <c r="P5">
+        <v>3</v>
       </c>
       <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5">
         <v>185</v>
       </c>
-      <c r="R5">
+      <c r="U5">
         <v>1</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1036,23 +1090,32 @@
       <c r="O6">
         <v>4</v>
       </c>
-      <c r="P6" t="s">
-        <v>23</v>
+      <c r="P6">
+        <v>4</v>
       </c>
       <c r="Q6">
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6">
         <v>203</v>
       </c>
-      <c r="R6">
+      <c r="U6">
         <v>2</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1098,23 +1161,32 @@
       <c r="O7">
         <v>5</v>
       </c>
-      <c r="P7" t="s">
-        <v>24</v>
+      <c r="P7">
+        <v>5</v>
       </c>
       <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T7">
         <v>229</v>
       </c>
-      <c r="R7">
+      <c r="U7">
         <v>2</v>
       </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1160,23 +1232,32 @@
       <c r="O8">
         <v>6</v>
       </c>
-      <c r="P8" t="s">
-        <v>25</v>
+      <c r="P8">
+        <v>6</v>
       </c>
       <c r="Q8">
+        <v>6</v>
+      </c>
+      <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="S8" t="s">
+        <v>28</v>
+      </c>
+      <c r="T8">
         <v>445</v>
       </c>
-      <c r="R8">
+      <c r="U8">
         <v>2</v>
       </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1222,23 +1303,32 @@
       <c r="O9">
         <v>7</v>
       </c>
-      <c r="P9" t="s">
-        <v>26</v>
+      <c r="P9">
+        <v>7</v>
       </c>
       <c r="Q9">
+        <v>7</v>
+      </c>
+      <c r="R9">
+        <v>7</v>
+      </c>
+      <c r="S9" t="s">
+        <v>29</v>
+      </c>
+      <c r="T9">
         <v>526</v>
       </c>
-      <c r="R9">
+      <c r="U9">
         <v>3</v>
       </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1284,23 +1374,32 @@
       <c r="O10">
         <v>8</v>
       </c>
-      <c r="P10" t="s">
-        <v>27</v>
+      <c r="P10">
+        <v>8</v>
       </c>
       <c r="Q10">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>8</v>
+      </c>
+      <c r="S10" t="s">
+        <v>30</v>
+      </c>
+      <c r="T10">
         <v>563</v>
       </c>
-      <c r="R10">
+      <c r="U10">
         <v>5</v>
       </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1346,23 +1445,32 @@
       <c r="O11">
         <v>9</v>
       </c>
-      <c r="P11" t="s">
-        <v>28</v>
+      <c r="P11">
+        <v>9</v>
       </c>
       <c r="Q11">
+        <v>9</v>
+      </c>
+      <c r="R11">
+        <v>9</v>
+      </c>
+      <c r="S11" t="s">
+        <v>31</v>
+      </c>
+      <c r="T11">
         <v>680</v>
       </c>
-      <c r="R11">
+      <c r="U11">
         <v>6</v>
       </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1408,23 +1516,32 @@
       <c r="O12">
         <v>10</v>
       </c>
-      <c r="P12" t="s">
-        <v>29</v>
+      <c r="P12">
+        <v>10</v>
       </c>
       <c r="Q12">
+        <v>10</v>
+      </c>
+      <c r="R12">
+        <v>10</v>
+      </c>
+      <c r="S12" t="s">
+        <v>32</v>
+      </c>
+      <c r="T12">
         <v>847</v>
       </c>
-      <c r="R12">
+      <c r="U12">
         <v>6</v>
       </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1470,23 +1587,32 @@
       <c r="O13">
         <v>11</v>
       </c>
-      <c r="P13" t="s">
-        <v>30</v>
+      <c r="P13">
+        <v>11</v>
       </c>
       <c r="Q13">
+        <v>11</v>
+      </c>
+      <c r="R13">
+        <v>11</v>
+      </c>
+      <c r="S13" t="s">
+        <v>33</v>
+      </c>
+      <c r="T13">
         <v>955</v>
       </c>
-      <c r="R13">
+      <c r="U13">
         <v>6</v>
       </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1532,23 +1658,32 @@
       <c r="O14">
         <v>12</v>
       </c>
-      <c r="P14" t="s">
-        <v>31</v>
+      <c r="P14">
+        <v>12</v>
       </c>
       <c r="Q14">
+        <v>12</v>
+      </c>
+      <c r="R14">
+        <v>12</v>
+      </c>
+      <c r="S14" t="s">
+        <v>34</v>
+      </c>
+      <c r="T14">
         <v>1106</v>
       </c>
-      <c r="R14">
+      <c r="U14">
         <v>13</v>
       </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1594,23 +1729,32 @@
       <c r="O15">
         <v>13</v>
       </c>
-      <c r="P15" t="s">
-        <v>32</v>
+      <c r="P15">
+        <v>13</v>
       </c>
       <c r="Q15">
+        <v>13</v>
+      </c>
+      <c r="R15">
+        <v>13</v>
+      </c>
+      <c r="S15" t="s">
+        <v>35</v>
+      </c>
+      <c r="T15">
         <v>1284</v>
       </c>
-      <c r="R15">
+      <c r="U15">
         <v>17</v>
       </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1656,23 +1800,32 @@
       <c r="O16">
         <v>14</v>
       </c>
-      <c r="P16" t="s">
-        <v>33</v>
+      <c r="P16">
+        <v>14</v>
       </c>
       <c r="Q16">
+        <v>14</v>
+      </c>
+      <c r="R16">
+        <v>14</v>
+      </c>
+      <c r="S16" t="s">
+        <v>36</v>
+      </c>
+      <c r="T16">
         <v>1395</v>
       </c>
-      <c r="R16">
+      <c r="U16">
         <v>20</v>
       </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1718,23 +1871,32 @@
       <c r="O17">
         <v>15</v>
       </c>
-      <c r="P17" t="s">
-        <v>34</v>
+      <c r="P17">
+        <v>15</v>
       </c>
       <c r="Q17">
+        <v>15</v>
+      </c>
+      <c r="R17">
+        <v>15</v>
+      </c>
+      <c r="S17" t="s">
+        <v>37</v>
+      </c>
+      <c r="T17">
         <v>1809</v>
       </c>
-      <c r="R17">
+      <c r="U17">
         <v>22</v>
       </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1780,23 +1942,32 @@
       <c r="O18">
         <v>16</v>
       </c>
-      <c r="P18" t="s">
-        <v>35</v>
+      <c r="P18">
+        <v>16</v>
       </c>
       <c r="Q18">
+        <v>16</v>
+      </c>
+      <c r="R18">
+        <v>16</v>
+      </c>
+      <c r="S18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T18">
         <v>2146</v>
       </c>
-      <c r="R18">
+      <c r="U18">
         <v>23</v>
       </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1842,23 +2013,32 @@
       <c r="O19">
         <v>17</v>
       </c>
-      <c r="P19" t="s">
-        <v>36</v>
+      <c r="P19">
+        <v>17</v>
       </c>
       <c r="Q19">
+        <v>17</v>
+      </c>
+      <c r="R19">
+        <v>17</v>
+      </c>
+      <c r="S19" t="s">
+        <v>39</v>
+      </c>
+      <c r="T19">
         <v>2341</v>
       </c>
-      <c r="R19">
+      <c r="U19">
         <v>31</v>
       </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1904,23 +2084,32 @@
       <c r="O20">
         <v>18</v>
       </c>
-      <c r="P20" t="s">
-        <v>37</v>
+      <c r="P20">
+        <v>18</v>
       </c>
       <c r="Q20">
+        <v>18</v>
+      </c>
+      <c r="R20">
+        <v>18</v>
+      </c>
+      <c r="S20" t="s">
+        <v>40</v>
+      </c>
+      <c r="T20">
         <v>3047</v>
       </c>
-      <c r="R20">
+      <c r="U20">
         <v>34</v>
       </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1966,23 +2155,32 @@
       <c r="O21">
         <v>19</v>
       </c>
-      <c r="P21" t="s">
-        <v>38</v>
+      <c r="P21">
+        <v>19</v>
       </c>
       <c r="Q21">
+        <v>19</v>
+      </c>
+      <c r="R21">
+        <v>19</v>
+      </c>
+      <c r="S21" t="s">
+        <v>41</v>
+      </c>
+      <c r="T21">
         <v>3261</v>
       </c>
-      <c r="R21">
+      <c r="U21">
         <v>40</v>
       </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2028,23 +2226,32 @@
       <c r="O22">
         <v>20</v>
       </c>
-      <c r="P22" t="s">
-        <v>39</v>
+      <c r="P22">
+        <v>20</v>
       </c>
       <c r="Q22">
+        <v>20</v>
+      </c>
+      <c r="R22">
+        <v>20</v>
+      </c>
+      <c r="S22" t="s">
+        <v>42</v>
+      </c>
+      <c r="T22">
         <v>3561</v>
       </c>
-      <c r="R22">
+      <c r="U22">
         <v>41</v>
       </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2090,23 +2297,32 @@
       <c r="O23">
         <v>21</v>
       </c>
-      <c r="P23" t="s">
-        <v>40</v>
+      <c r="P23">
+        <v>21</v>
       </c>
       <c r="Q23">
+        <v>21</v>
+      </c>
+      <c r="R23">
+        <v>21</v>
+      </c>
+      <c r="S23" t="s">
+        <v>43</v>
+      </c>
+      <c r="T23">
         <v>3629</v>
       </c>
-      <c r="R23">
+      <c r="U23">
         <v>44</v>
       </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="T23">
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
         <v>3585</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:23">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2152,23 +2368,32 @@
       <c r="O24">
         <v>22</v>
       </c>
-      <c r="P24" t="s">
-        <v>41</v>
+      <c r="P24">
+        <v>22</v>
       </c>
       <c r="Q24">
+        <v>22</v>
+      </c>
+      <c r="R24">
+        <v>22</v>
+      </c>
+      <c r="S24" t="s">
+        <v>44</v>
+      </c>
+      <c r="T24">
         <v>3744</v>
       </c>
-      <c r="R24">
+      <c r="U24">
         <v>46</v>
       </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24">
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
         <v>3698</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:23">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2214,23 +2439,32 @@
       <c r="O25">
         <v>23</v>
       </c>
-      <c r="P25" t="s">
-        <v>42</v>
+      <c r="P25">
+        <v>23</v>
       </c>
       <c r="Q25">
+        <v>23</v>
+      </c>
+      <c r="R25">
+        <v>23</v>
+      </c>
+      <c r="S25" t="s">
+        <v>45</v>
+      </c>
+      <c r="T25">
         <v>3907</v>
       </c>
-      <c r="R25">
+      <c r="U25">
         <v>52</v>
       </c>
-      <c r="S25">
-        <v>0</v>
-      </c>
-      <c r="T25">
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
         <v>3855</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:23">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2276,23 +2510,32 @@
       <c r="O26">
         <v>24</v>
       </c>
-      <c r="P26" t="s">
-        <v>43</v>
+      <c r="P26">
+        <v>24</v>
       </c>
       <c r="Q26">
+        <v>24</v>
+      </c>
+      <c r="R26">
+        <v>24</v>
+      </c>
+      <c r="S26" t="s">
+        <v>46</v>
+      </c>
+      <c r="T26">
         <v>4097</v>
       </c>
-      <c r="R26">
+      <c r="U26">
         <v>58</v>
       </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
-      <c r="T26">
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
         <v>4039</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:23">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2338,23 +2581,32 @@
       <c r="O27">
         <v>25</v>
       </c>
-      <c r="P27" t="s">
-        <v>44</v>
+      <c r="P27">
+        <v>25</v>
       </c>
       <c r="Q27">
+        <v>25</v>
+      </c>
+      <c r="R27">
+        <v>25</v>
+      </c>
+      <c r="S27" t="s">
+        <v>47</v>
+      </c>
+      <c r="T27">
         <v>4306</v>
       </c>
-      <c r="R27">
+      <c r="U27">
         <v>63</v>
       </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
-      <c r="T27">
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
         <v>4243</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:23">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2400,23 +2652,32 @@
       <c r="O28">
         <v>26</v>
       </c>
-      <c r="P28" t="s">
-        <v>45</v>
+      <c r="P28">
+        <v>26</v>
       </c>
       <c r="Q28">
+        <v>26</v>
+      </c>
+      <c r="R28">
+        <v>26</v>
+      </c>
+      <c r="S28" t="s">
+        <v>48</v>
+      </c>
+      <c r="T28">
         <v>4460</v>
       </c>
-      <c r="R28">
+      <c r="U28">
         <v>67</v>
       </c>
-      <c r="S28">
-        <v>0</v>
-      </c>
-      <c r="T28">
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
         <v>4393</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:23">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2462,23 +2723,32 @@
       <c r="O29">
         <v>27</v>
       </c>
-      <c r="P29" t="s">
-        <v>46</v>
+      <c r="P29">
+        <v>27</v>
       </c>
       <c r="Q29">
+        <v>27</v>
+      </c>
+      <c r="R29">
+        <v>27</v>
+      </c>
+      <c r="S29" t="s">
+        <v>49</v>
+      </c>
+      <c r="T29">
         <v>4653</v>
       </c>
-      <c r="R29">
+      <c r="U29">
         <v>71</v>
       </c>
-      <c r="S29">
-        <v>0</v>
-      </c>
-      <c r="T29">
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
         <v>4582</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:23">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2524,23 +2794,32 @@
       <c r="O30">
         <v>28</v>
       </c>
-      <c r="P30" t="s">
-        <v>47</v>
+      <c r="P30">
+        <v>28</v>
       </c>
       <c r="Q30">
+        <v>28</v>
+      </c>
+      <c r="R30">
+        <v>28</v>
+      </c>
+      <c r="S30" t="s">
+        <v>50</v>
+      </c>
+      <c r="T30">
         <v>4823</v>
       </c>
-      <c r="R30">
+      <c r="U30">
         <v>75</v>
       </c>
-      <c r="S30">
-        <v>0</v>
-      </c>
-      <c r="T30">
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
         <v>4748</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:23">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2586,23 +2865,32 @@
       <c r="O31">
         <v>29</v>
       </c>
-      <c r="P31" t="s">
-        <v>48</v>
+      <c r="P31">
+        <v>29</v>
       </c>
       <c r="Q31">
+        <v>29</v>
+      </c>
+      <c r="R31">
+        <v>29</v>
+      </c>
+      <c r="S31" t="s">
+        <v>51</v>
+      </c>
+      <c r="T31">
         <v>4977</v>
       </c>
-      <c r="R31">
+      <c r="U31">
         <v>78</v>
       </c>
-      <c r="S31">
-        <v>0</v>
-      </c>
-      <c r="T31">
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
         <v>4899</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:23">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2648,23 +2936,32 @@
       <c r="O32">
         <v>30</v>
       </c>
-      <c r="P32" t="s">
-        <v>49</v>
+      <c r="P32">
+        <v>30</v>
       </c>
       <c r="Q32">
+        <v>30</v>
+      </c>
+      <c r="R32">
+        <v>30</v>
+      </c>
+      <c r="S32" t="s">
+        <v>52</v>
+      </c>
+      <c r="T32">
         <v>5143</v>
       </c>
-      <c r="R32">
+      <c r="U32">
         <v>79</v>
       </c>
-      <c r="S32">
-        <v>0</v>
-      </c>
-      <c r="T32">
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
         <v>5064</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:23">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2710,23 +3007,32 @@
       <c r="O33">
         <v>31</v>
       </c>
-      <c r="P33" t="s">
-        <v>50</v>
+      <c r="P33">
+        <v>31</v>
       </c>
       <c r="Q33">
+        <v>31</v>
+      </c>
+      <c r="R33">
+        <v>31</v>
+      </c>
+      <c r="S33" t="s">
+        <v>53</v>
+      </c>
+      <c r="T33">
         <v>5211</v>
       </c>
-      <c r="R33">
+      <c r="U33">
         <v>80</v>
       </c>
-      <c r="S33">
-        <v>0</v>
-      </c>
-      <c r="T33">
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
         <v>5131</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:23">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2772,23 +3078,32 @@
       <c r="O34">
         <v>32</v>
       </c>
-      <c r="P34" t="s">
-        <v>51</v>
+      <c r="P34">
+        <v>32</v>
       </c>
       <c r="Q34">
+        <v>32</v>
+      </c>
+      <c r="R34">
+        <v>32</v>
+      </c>
+      <c r="S34" t="s">
+        <v>54</v>
+      </c>
+      <c r="T34">
         <v>5330</v>
       </c>
-      <c r="R34">
+      <c r="U34">
         <v>82</v>
       </c>
-      <c r="S34">
-        <v>0</v>
-      </c>
-      <c r="T34">
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
         <v>5248</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:23">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2834,23 +3149,32 @@
       <c r="O35">
         <v>33</v>
       </c>
-      <c r="P35" t="s">
-        <v>52</v>
+      <c r="P35">
+        <v>33</v>
       </c>
       <c r="Q35">
+        <v>33</v>
+      </c>
+      <c r="R35">
+        <v>33</v>
+      </c>
+      <c r="S35" t="s">
+        <v>55</v>
+      </c>
+      <c r="T35">
         <v>5482</v>
       </c>
-      <c r="R35">
+      <c r="U35">
         <v>84</v>
       </c>
-      <c r="S35">
-        <v>0</v>
-      </c>
-      <c r="T35">
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
         <v>5398</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:23">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2896,23 +3220,32 @@
       <c r="O36">
         <v>34</v>
       </c>
-      <c r="P36" t="s">
-        <v>53</v>
+      <c r="P36">
+        <v>34</v>
       </c>
       <c r="Q36">
+        <v>34</v>
+      </c>
+      <c r="R36">
+        <v>34</v>
+      </c>
+      <c r="S36" t="s">
+        <v>56</v>
+      </c>
+      <c r="T36">
         <v>5482</v>
       </c>
-      <c r="R36">
+      <c r="U36">
         <v>84</v>
       </c>
-      <c r="S36">
-        <v>0</v>
-      </c>
-      <c r="T36">
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
         <v>5398</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:23">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2958,23 +3291,32 @@
       <c r="O37">
         <v>35</v>
       </c>
-      <c r="P37" t="s">
-        <v>54</v>
+      <c r="P37">
+        <v>35</v>
       </c>
       <c r="Q37">
+        <v>35</v>
+      </c>
+      <c r="R37">
+        <v>35</v>
+      </c>
+      <c r="S37" t="s">
+        <v>57</v>
+      </c>
+      <c r="T37">
         <v>5628</v>
       </c>
-      <c r="R37">
+      <c r="U37">
         <v>84</v>
       </c>
-      <c r="S37">
-        <v>0</v>
-      </c>
-      <c r="T37">
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
         <v>5544</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:23">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3020,23 +3362,32 @@
       <c r="O38">
         <v>36</v>
       </c>
-      <c r="P38" t="s">
-        <v>55</v>
+      <c r="P38">
+        <v>36</v>
       </c>
       <c r="Q38">
+        <v>36</v>
+      </c>
+      <c r="R38">
+        <v>36</v>
+      </c>
+      <c r="S38" t="s">
+        <v>58</v>
+      </c>
+      <c r="T38">
         <v>5628</v>
       </c>
-      <c r="R38">
+      <c r="U38">
         <v>84</v>
       </c>
-      <c r="S38">
-        <v>0</v>
-      </c>
-      <c r="T38">
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
         <v>5544</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:23">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3082,23 +3433,32 @@
       <c r="O39">
         <v>37</v>
       </c>
-      <c r="P39" t="s">
-        <v>56</v>
+      <c r="P39">
+        <v>37</v>
       </c>
       <c r="Q39">
+        <v>37</v>
+      </c>
+      <c r="R39">
+        <v>37</v>
+      </c>
+      <c r="S39" t="s">
+        <v>59</v>
+      </c>
+      <c r="T39">
         <v>5827</v>
       </c>
-      <c r="R39">
+      <c r="U39">
         <v>98</v>
       </c>
-      <c r="S39">
-        <v>0</v>
-      </c>
-      <c r="T39">
+      <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
         <v>5729</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:23">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3144,23 +3504,32 @@
       <c r="O40">
         <v>38</v>
       </c>
-      <c r="P40" t="s">
-        <v>57</v>
+      <c r="P40">
+        <v>38</v>
       </c>
       <c r="Q40">
+        <v>38</v>
+      </c>
+      <c r="R40">
+        <v>38</v>
+      </c>
+      <c r="S40" t="s">
+        <v>60</v>
+      </c>
+      <c r="T40">
         <v>6161</v>
       </c>
-      <c r="R40">
+      <c r="U40">
         <v>109</v>
       </c>
-      <c r="S40">
-        <v>0</v>
-      </c>
-      <c r="T40">
+      <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40">
         <v>6052</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:23">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3206,23 +3575,32 @@
       <c r="O41">
         <v>39</v>
       </c>
-      <c r="P41" t="s">
-        <v>58</v>
+      <c r="P41">
+        <v>39</v>
       </c>
       <c r="Q41">
+        <v>39</v>
+      </c>
+      <c r="R41">
+        <v>39</v>
+      </c>
+      <c r="S41" t="s">
+        <v>61</v>
+      </c>
+      <c r="T41">
         <v>6356</v>
       </c>
-      <c r="R41">
+      <c r="U41">
         <v>114</v>
       </c>
-      <c r="S41">
-        <v>0</v>
-      </c>
-      <c r="T41">
+      <c r="V41">
+        <v>0</v>
+      </c>
+      <c r="W41">
         <v>6242</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:23">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3268,23 +3646,32 @@
       <c r="O42">
         <v>40</v>
       </c>
-      <c r="P42" t="s">
-        <v>59</v>
+      <c r="P42">
+        <v>40</v>
       </c>
       <c r="Q42">
+        <v>40</v>
+      </c>
+      <c r="R42">
+        <v>40</v>
+      </c>
+      <c r="S42" t="s">
+        <v>62</v>
+      </c>
+      <c r="T42">
         <v>6551</v>
       </c>
-      <c r="R42">
+      <c r="U42">
         <v>122</v>
       </c>
-      <c r="S42">
-        <v>0</v>
-      </c>
-      <c r="T42">
+      <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42">
         <v>6429</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:23">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3330,23 +3717,32 @@
       <c r="O43">
         <v>41</v>
       </c>
-      <c r="P43" t="s">
-        <v>60</v>
+      <c r="P43">
+        <v>41</v>
       </c>
       <c r="Q43">
+        <v>41</v>
+      </c>
+      <c r="R43">
+        <v>41</v>
+      </c>
+      <c r="S43" t="s">
+        <v>63</v>
+      </c>
+      <c r="T43">
         <v>6708</v>
       </c>
-      <c r="R43">
+      <c r="U43">
         <v>129</v>
       </c>
-      <c r="S43">
-        <v>0</v>
-      </c>
-      <c r="T43">
+      <c r="V43">
+        <v>0</v>
+      </c>
+      <c r="W43">
         <v>6579</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:23">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3392,23 +3788,32 @@
       <c r="O44">
         <v>42</v>
       </c>
-      <c r="P44" t="s">
-        <v>61</v>
+      <c r="P44">
+        <v>42</v>
       </c>
       <c r="Q44">
+        <v>42</v>
+      </c>
+      <c r="R44">
+        <v>42</v>
+      </c>
+      <c r="S44" t="s">
+        <v>64</v>
+      </c>
+      <c r="T44">
         <v>6838</v>
       </c>
-      <c r="R44">
+      <c r="U44">
         <v>133</v>
       </c>
-      <c r="S44">
-        <v>0</v>
-      </c>
-      <c r="T44">
+      <c r="V44">
+        <v>0</v>
+      </c>
+      <c r="W44">
         <v>6705</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:23">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3454,23 +3859,32 @@
       <c r="O45">
         <v>43</v>
       </c>
-      <c r="P45" t="s">
-        <v>62</v>
+      <c r="P45">
+        <v>43</v>
       </c>
       <c r="Q45">
+        <v>43</v>
+      </c>
+      <c r="R45">
+        <v>43</v>
+      </c>
+      <c r="S45" t="s">
+        <v>65</v>
+      </c>
+      <c r="T45">
         <v>6967</v>
       </c>
-      <c r="R45">
+      <c r="U45">
         <v>140</v>
       </c>
-      <c r="S45">
-        <v>0</v>
-      </c>
-      <c r="T45">
+      <c r="V45">
+        <v>0</v>
+      </c>
+      <c r="W45">
         <v>6827</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:23">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3516,23 +3930,32 @@
       <c r="O46">
         <v>44</v>
       </c>
-      <c r="P46" t="s">
-        <v>63</v>
+      <c r="P46">
+        <v>44</v>
       </c>
       <c r="Q46">
+        <v>44</v>
+      </c>
+      <c r="R46">
+        <v>44</v>
+      </c>
+      <c r="S46" t="s">
+        <v>66</v>
+      </c>
+      <c r="T46">
         <v>7128</v>
       </c>
-      <c r="R46">
+      <c r="U46">
         <v>144</v>
       </c>
-      <c r="S46">
-        <v>0</v>
-      </c>
-      <c r="T46">
+      <c r="V46">
+        <v>0</v>
+      </c>
+      <c r="W46">
         <v>6984</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:23">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3578,23 +4001,32 @@
       <c r="O47">
         <v>45</v>
       </c>
-      <c r="P47" t="s">
-        <v>64</v>
+      <c r="P47">
+        <v>45</v>
       </c>
       <c r="Q47">
+        <v>45</v>
+      </c>
+      <c r="R47">
+        <v>45</v>
+      </c>
+      <c r="S47" t="s">
+        <v>67</v>
+      </c>
+      <c r="T47">
         <v>7244</v>
       </c>
-      <c r="R47">
+      <c r="U47">
         <v>150</v>
       </c>
-      <c r="S47">
-        <v>0</v>
-      </c>
-      <c r="T47">
+      <c r="V47">
+        <v>0</v>
+      </c>
+      <c r="W47">
         <v>7094</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:23">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3640,23 +4072,32 @@
       <c r="O48">
         <v>46</v>
       </c>
-      <c r="P48" t="s">
-        <v>65</v>
+      <c r="P48">
+        <v>46</v>
       </c>
       <c r="Q48">
+        <v>46</v>
+      </c>
+      <c r="R48">
+        <v>46</v>
+      </c>
+      <c r="S48" t="s">
+        <v>68</v>
+      </c>
+      <c r="T48">
         <v>7377</v>
       </c>
-      <c r="R48">
+      <c r="U48">
         <v>154</v>
       </c>
-      <c r="S48">
-        <v>0</v>
-      </c>
-      <c r="T48">
+      <c r="V48">
+        <v>0</v>
+      </c>
+      <c r="W48">
         <v>7223</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:23">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3702,23 +4143,32 @@
       <c r="O49">
         <v>47</v>
       </c>
-      <c r="P49" t="s">
-        <v>66</v>
+      <c r="P49">
+        <v>47</v>
       </c>
       <c r="Q49">
+        <v>47</v>
+      </c>
+      <c r="R49">
+        <v>47</v>
+      </c>
+      <c r="S49" t="s">
+        <v>69</v>
+      </c>
+      <c r="T49">
         <v>7594</v>
       </c>
-      <c r="R49">
+      <c r="U49">
         <v>160</v>
       </c>
-      <c r="S49">
-        <v>0</v>
-      </c>
-      <c r="T49">
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
         <v>7434</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:23">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3764,23 +4214,32 @@
       <c r="O50">
         <v>48</v>
       </c>
-      <c r="P50" t="s">
-        <v>67</v>
+      <c r="P50">
+        <v>48</v>
       </c>
       <c r="Q50">
+        <v>48</v>
+      </c>
+      <c r="R50">
+        <v>48</v>
+      </c>
+      <c r="S50" t="s">
+        <v>70</v>
+      </c>
+      <c r="T50">
         <v>7803</v>
       </c>
-      <c r="R50">
+      <c r="U50">
         <v>168</v>
       </c>
-      <c r="S50">
-        <v>0</v>
-      </c>
-      <c r="T50">
+      <c r="V50">
+        <v>0</v>
+      </c>
+      <c r="W50">
         <v>7635</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:23">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3826,23 +4285,32 @@
       <c r="O51">
         <v>49</v>
       </c>
-      <c r="P51" t="s">
-        <v>68</v>
+      <c r="P51">
+        <v>49</v>
       </c>
       <c r="Q51">
+        <v>49</v>
+      </c>
+      <c r="R51">
+        <v>49</v>
+      </c>
+      <c r="S51" t="s">
+        <v>71</v>
+      </c>
+      <c r="T51">
         <v>7878</v>
       </c>
-      <c r="R51">
+      <c r="U51">
         <v>172</v>
       </c>
-      <c r="S51">
-        <v>0</v>
-      </c>
-      <c r="T51">
+      <c r="V51">
+        <v>0</v>
+      </c>
+      <c r="W51">
         <v>7706</v>
       </c>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:23">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3888,23 +4356,32 @@
       <c r="O52">
         <v>50</v>
       </c>
-      <c r="P52" t="s">
-        <v>69</v>
+      <c r="P52">
+        <v>50</v>
       </c>
       <c r="Q52">
+        <v>50</v>
+      </c>
+      <c r="R52">
+        <v>50</v>
+      </c>
+      <c r="S52" t="s">
+        <v>72</v>
+      </c>
+      <c r="T52">
         <v>8176</v>
       </c>
-      <c r="R52">
+      <c r="U52">
         <v>179</v>
       </c>
-      <c r="S52">
-        <v>0</v>
-      </c>
-      <c r="T52">
+      <c r="V52">
+        <v>0</v>
+      </c>
+      <c r="W52">
         <v>7997</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:23">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3950,23 +4427,32 @@
       <c r="O53">
         <v>51</v>
       </c>
-      <c r="P53" t="s">
-        <v>70</v>
+      <c r="P53">
+        <v>51</v>
       </c>
       <c r="Q53">
+        <v>51</v>
+      </c>
+      <c r="R53">
+        <v>51</v>
+      </c>
+      <c r="S53" t="s">
+        <v>73</v>
+      </c>
+      <c r="T53">
         <v>8416</v>
       </c>
-      <c r="R53">
+      <c r="U53">
         <v>183</v>
       </c>
-      <c r="S53">
-        <v>0</v>
-      </c>
-      <c r="T53">
+      <c r="V53">
+        <v>0</v>
+      </c>
+      <c r="W53">
         <v>8233</v>
       </c>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:23">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4012,23 +4498,32 @@
       <c r="O54">
         <v>52</v>
       </c>
-      <c r="P54" t="s">
-        <v>71</v>
+      <c r="P54">
+        <v>52</v>
       </c>
       <c r="Q54">
+        <v>52</v>
+      </c>
+      <c r="R54">
+        <v>52</v>
+      </c>
+      <c r="S54" t="s">
+        <v>74</v>
+      </c>
+      <c r="T54">
         <v>8621</v>
       </c>
-      <c r="R54">
+      <c r="U54">
         <v>188</v>
       </c>
-      <c r="S54">
-        <v>0</v>
-      </c>
-      <c r="T54">
+      <c r="V54">
+        <v>0</v>
+      </c>
+      <c r="W54">
         <v>8433</v>
       </c>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:23">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4074,23 +4569,32 @@
       <c r="O55">
         <v>53</v>
       </c>
-      <c r="P55" t="s">
-        <v>72</v>
+      <c r="P55">
+        <v>53</v>
       </c>
       <c r="Q55">
+        <v>53</v>
+      </c>
+      <c r="R55">
+        <v>53</v>
+      </c>
+      <c r="S55" t="s">
+        <v>75</v>
+      </c>
+      <c r="T55">
         <v>8817</v>
       </c>
-      <c r="R55">
+      <c r="U55">
         <v>193</v>
       </c>
-      <c r="S55">
-        <v>0</v>
-      </c>
-      <c r="T55">
+      <c r="V55">
+        <v>0</v>
+      </c>
+      <c r="W55">
         <v>8624</v>
       </c>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:23">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4136,23 +4640,32 @@
       <c r="O56">
         <v>54</v>
       </c>
-      <c r="P56" t="s">
-        <v>73</v>
+      <c r="P56">
+        <v>54</v>
       </c>
       <c r="Q56">
+        <v>54</v>
+      </c>
+      <c r="R56">
+        <v>54</v>
+      </c>
+      <c r="S56" t="s">
+        <v>76</v>
+      </c>
+      <c r="T56">
         <v>9050</v>
       </c>
-      <c r="R56">
+      <c r="U56">
         <v>193</v>
       </c>
-      <c r="S56">
-        <v>0</v>
-      </c>
-      <c r="T56">
+      <c r="V56">
+        <v>0</v>
+      </c>
+      <c r="W56">
         <v>8857</v>
       </c>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:23">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4198,23 +4711,32 @@
       <c r="O57">
         <v>55</v>
       </c>
-      <c r="P57" t="s">
-        <v>74</v>
+      <c r="P57">
+        <v>55</v>
       </c>
       <c r="Q57">
+        <v>55</v>
+      </c>
+      <c r="R57">
+        <v>55</v>
+      </c>
+      <c r="S57" t="s">
+        <v>77</v>
+      </c>
+      <c r="T57">
         <v>9126</v>
       </c>
-      <c r="R57">
+      <c r="U57">
         <v>204</v>
       </c>
-      <c r="S57">
-        <v>0</v>
-      </c>
-      <c r="T57">
+      <c r="V57">
+        <v>0</v>
+      </c>
+      <c r="W57">
         <v>8922</v>
       </c>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:23">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4260,23 +4782,32 @@
       <c r="O58">
         <v>56</v>
       </c>
-      <c r="P58" t="s">
-        <v>75</v>
+      <c r="P58">
+        <v>56</v>
       </c>
       <c r="Q58">
+        <v>56</v>
+      </c>
+      <c r="R58">
+        <v>56</v>
+      </c>
+      <c r="S58" t="s">
+        <v>78</v>
+      </c>
+      <c r="T58">
         <v>9465</v>
       </c>
-      <c r="R58">
+      <c r="U58">
         <v>204</v>
       </c>
-      <c r="S58">
-        <v>0</v>
-      </c>
-      <c r="T58">
+      <c r="V58">
+        <v>0</v>
+      </c>
+      <c r="W58">
         <v>9261</v>
       </c>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:23">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4322,23 +4853,32 @@
       <c r="O59">
         <v>57</v>
       </c>
-      <c r="P59" t="s">
-        <v>76</v>
+      <c r="P59">
+        <v>57</v>
       </c>
       <c r="Q59">
+        <v>57</v>
+      </c>
+      <c r="R59">
+        <v>57</v>
+      </c>
+      <c r="S59" t="s">
+        <v>79</v>
+      </c>
+      <c r="T59">
         <v>9635</v>
       </c>
-      <c r="R59">
+      <c r="U59">
         <v>205</v>
       </c>
-      <c r="S59">
-        <v>0</v>
-      </c>
-      <c r="T59">
+      <c r="V59">
+        <v>0</v>
+      </c>
+      <c r="W59">
         <v>9430</v>
       </c>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:23">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4384,23 +4924,32 @@
       <c r="O60">
         <v>58</v>
       </c>
-      <c r="P60" t="s">
-        <v>77</v>
+      <c r="P60">
+        <v>58</v>
       </c>
       <c r="Q60">
+        <v>58</v>
+      </c>
+      <c r="R60">
+        <v>58</v>
+      </c>
+      <c r="S60" t="s">
+        <v>80</v>
+      </c>
+      <c r="T60">
         <v>9859</v>
       </c>
-      <c r="R60">
+      <c r="U60">
         <v>207</v>
       </c>
-      <c r="S60">
-        <v>0</v>
-      </c>
-      <c r="T60">
+      <c r="V60">
+        <v>0</v>
+      </c>
+      <c r="W60">
         <v>9652</v>
       </c>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:23">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -4446,23 +4995,32 @@
       <c r="O61">
         <v>59</v>
       </c>
-      <c r="P61" t="s">
-        <v>78</v>
+      <c r="P61">
+        <v>59</v>
       </c>
       <c r="Q61">
+        <v>59</v>
+      </c>
+      <c r="R61">
+        <v>59</v>
+      </c>
+      <c r="S61" t="s">
+        <v>81</v>
+      </c>
+      <c r="T61">
         <v>10095</v>
       </c>
-      <c r="R61">
+      <c r="U61">
         <v>210</v>
       </c>
-      <c r="S61">
-        <v>0</v>
-      </c>
-      <c r="T61">
+      <c r="V61">
+        <v>0</v>
+      </c>
+      <c r="W61">
         <v>9885</v>
       </c>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:23">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4508,23 +5066,32 @@
       <c r="O62">
         <v>60</v>
       </c>
-      <c r="P62" t="s">
-        <v>79</v>
+      <c r="P62">
+        <v>60</v>
       </c>
       <c r="Q62">
+        <v>60</v>
+      </c>
+      <c r="R62">
+        <v>60</v>
+      </c>
+      <c r="S62" t="s">
+        <v>82</v>
+      </c>
+      <c r="T62">
         <v>10283</v>
       </c>
-      <c r="R62">
+      <c r="U62">
         <v>216</v>
       </c>
-      <c r="S62">
-        <v>0</v>
-      </c>
-      <c r="T62">
+      <c r="V62">
+        <v>0</v>
+      </c>
+      <c r="W62">
         <v>10067</v>
       </c>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:23">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4570,23 +5137,32 @@
       <c r="O63">
         <v>61</v>
       </c>
-      <c r="P63" t="s">
-        <v>80</v>
+      <c r="P63">
+        <v>61</v>
       </c>
       <c r="Q63">
+        <v>61</v>
+      </c>
+      <c r="R63">
+        <v>61</v>
+      </c>
+      <c r="S63" t="s">
+        <v>83</v>
+      </c>
+      <c r="T63">
         <v>10526</v>
       </c>
-      <c r="R63">
+      <c r="U63">
         <v>217</v>
       </c>
-      <c r="S63">
-        <v>0</v>
-      </c>
-      <c r="T63">
+      <c r="V63">
+        <v>0</v>
+      </c>
+      <c r="W63">
         <v>10309</v>
       </c>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:23">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4632,23 +5208,32 @@
       <c r="O64">
         <v>62</v>
       </c>
-      <c r="P64" t="s">
-        <v>81</v>
+      <c r="P64">
+        <v>62</v>
       </c>
       <c r="Q64">
+        <v>62</v>
+      </c>
+      <c r="R64">
+        <v>62</v>
+      </c>
+      <c r="S64" t="s">
+        <v>84</v>
+      </c>
+      <c r="T64">
         <v>10770</v>
       </c>
-      <c r="R64">
+      <c r="U64">
         <v>219</v>
       </c>
-      <c r="S64">
-        <v>0</v>
-      </c>
-      <c r="T64">
+      <c r="V64">
+        <v>0</v>
+      </c>
+      <c r="W64">
         <v>10551</v>
       </c>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:23">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -4694,23 +5279,32 @@
       <c r="O65">
         <v>63</v>
       </c>
-      <c r="P65" t="s">
-        <v>82</v>
+      <c r="P65">
+        <v>63</v>
       </c>
       <c r="Q65">
+        <v>63</v>
+      </c>
+      <c r="R65">
+        <v>63</v>
+      </c>
+      <c r="S65" t="s">
+        <v>85</v>
+      </c>
+      <c r="T65">
         <v>10921</v>
       </c>
-      <c r="R65">
+      <c r="U65">
         <v>220</v>
       </c>
-      <c r="S65">
-        <v>0</v>
-      </c>
-      <c r="T65">
+      <c r="V65">
+        <v>0</v>
+      </c>
+      <c r="W65">
         <v>10701</v>
       </c>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:23">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -4756,23 +5350,32 @@
       <c r="O66">
         <v>64</v>
       </c>
-      <c r="P66" t="s">
-        <v>83</v>
+      <c r="P66">
+        <v>64</v>
       </c>
       <c r="Q66">
+        <v>64</v>
+      </c>
+      <c r="R66">
+        <v>64</v>
+      </c>
+      <c r="S66" t="s">
+        <v>86</v>
+      </c>
+      <c r="T66">
         <v>10995</v>
       </c>
-      <c r="R66">
+      <c r="U66">
         <v>221</v>
       </c>
-      <c r="S66">
-        <v>0</v>
-      </c>
-      <c r="T66">
+      <c r="V66">
+        <v>0</v>
+      </c>
+      <c r="W66">
         <v>10774</v>
       </c>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:23">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -4818,23 +5421,32 @@
       <c r="O67">
         <v>65</v>
       </c>
-      <c r="P67" t="s">
-        <v>84</v>
+      <c r="P67">
+        <v>65</v>
       </c>
       <c r="Q67">
+        <v>65</v>
+      </c>
+      <c r="R67">
+        <v>65</v>
+      </c>
+      <c r="S67" t="s">
+        <v>87</v>
+      </c>
+      <c r="T67">
         <v>11281</v>
       </c>
-      <c r="R67">
+      <c r="U67">
         <v>221</v>
       </c>
-      <c r="S67">
-        <v>0</v>
-      </c>
-      <c r="T67">
+      <c r="V67">
+        <v>0</v>
+      </c>
+      <c r="W67">
         <v>11060</v>
       </c>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:23">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4880,23 +5492,32 @@
       <c r="O68">
         <v>66</v>
       </c>
-      <c r="P68" t="s">
-        <v>85</v>
+      <c r="P68">
+        <v>66</v>
       </c>
       <c r="Q68">
+        <v>66</v>
+      </c>
+      <c r="R68">
+        <v>66</v>
+      </c>
+      <c r="S68" t="s">
+        <v>88</v>
+      </c>
+      <c r="T68">
         <v>11542</v>
       </c>
-      <c r="R68">
+      <c r="U68">
         <v>223</v>
       </c>
-      <c r="S68">
-        <v>0</v>
-      </c>
-      <c r="T68">
+      <c r="V68">
+        <v>0</v>
+      </c>
+      <c r="W68">
         <v>11319</v>
       </c>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:23">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4942,23 +5563,32 @@
       <c r="O69">
         <v>67</v>
       </c>
-      <c r="P69" t="s">
-        <v>86</v>
+      <c r="P69">
+        <v>67</v>
       </c>
       <c r="Q69">
+        <v>67</v>
+      </c>
+      <c r="R69">
+        <v>67</v>
+      </c>
+      <c r="S69" t="s">
+        <v>89</v>
+      </c>
+      <c r="T69">
         <v>11770</v>
       </c>
-      <c r="R69">
+      <c r="U69">
         <v>224</v>
       </c>
-      <c r="S69">
-        <v>0</v>
-      </c>
-      <c r="T69">
+      <c r="V69">
+        <v>0</v>
+      </c>
+      <c r="W69">
         <v>11546</v>
       </c>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:23">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -5004,23 +5634,32 @@
       <c r="O70">
         <v>68</v>
       </c>
-      <c r="P70" t="s">
-        <v>87</v>
+      <c r="P70">
+        <v>68</v>
       </c>
       <c r="Q70">
+        <v>68</v>
+      </c>
+      <c r="R70">
+        <v>68</v>
+      </c>
+      <c r="S70" t="s">
+        <v>90</v>
+      </c>
+      <c r="T70">
         <v>12009</v>
       </c>
-      <c r="R70">
+      <c r="U70">
         <v>228</v>
       </c>
-      <c r="S70">
-        <v>0</v>
-      </c>
-      <c r="T70">
+      <c r="V70">
+        <v>0</v>
+      </c>
+      <c r="W70">
         <v>11781</v>
       </c>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:23">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -5066,23 +5705,32 @@
       <c r="O71">
         <v>69</v>
       </c>
-      <c r="P71" t="s">
-        <v>88</v>
+      <c r="P71">
+        <v>69</v>
       </c>
       <c r="Q71">
+        <v>69</v>
+      </c>
+      <c r="R71">
+        <v>69</v>
+      </c>
+      <c r="S71" t="s">
+        <v>91</v>
+      </c>
+      <c r="T71">
         <v>12220</v>
       </c>
-      <c r="R71">
+      <c r="U71">
         <v>231</v>
       </c>
-      <c r="S71">
-        <v>0</v>
-      </c>
-      <c r="T71">
+      <c r="V71">
+        <v>0</v>
+      </c>
+      <c r="W71">
         <v>11989</v>
       </c>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:23">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -5128,23 +5776,32 @@
       <c r="O72">
         <v>70</v>
       </c>
-      <c r="P72" t="s">
-        <v>89</v>
+      <c r="P72">
+        <v>70</v>
       </c>
       <c r="Q72">
+        <v>70</v>
+      </c>
+      <c r="R72">
+        <v>70</v>
+      </c>
+      <c r="S72" t="s">
+        <v>92</v>
+      </c>
+      <c r="T72">
         <v>12276</v>
       </c>
-      <c r="R72">
+      <c r="U72">
         <v>232</v>
       </c>
-      <c r="S72">
-        <v>0</v>
-      </c>
-      <c r="T72">
+      <c r="V72">
+        <v>0</v>
+      </c>
+      <c r="W72">
         <v>12044</v>
       </c>
     </row>
-    <row r="73" spans="1:20">
+    <row r="73" spans="1:23">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -5190,23 +5847,32 @@
       <c r="O73">
         <v>71</v>
       </c>
-      <c r="P73" t="s">
-        <v>90</v>
+      <c r="P73">
+        <v>71</v>
       </c>
       <c r="Q73">
+        <v>71</v>
+      </c>
+      <c r="R73">
+        <v>71</v>
+      </c>
+      <c r="S73" t="s">
+        <v>93</v>
+      </c>
+      <c r="T73">
         <v>12664</v>
       </c>
-      <c r="R73">
+      <c r="U73">
         <v>235</v>
       </c>
-      <c r="S73">
-        <v>0</v>
-      </c>
-      <c r="T73">
+      <c r="V73">
+        <v>0</v>
+      </c>
+      <c r="W73">
         <v>12429</v>
       </c>
     </row>
-    <row r="74" spans="1:20">
+    <row r="74" spans="1:23">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -5252,23 +5918,32 @@
       <c r="O74">
         <v>72</v>
       </c>
-      <c r="P74" t="s">
-        <v>91</v>
+      <c r="P74">
+        <v>72</v>
       </c>
       <c r="Q74">
+        <v>72</v>
+      </c>
+      <c r="R74">
+        <v>72</v>
+      </c>
+      <c r="S74" t="s">
+        <v>94</v>
+      </c>
+      <c r="T74">
         <v>13027</v>
       </c>
-      <c r="R74">
+      <c r="U74">
         <v>236</v>
       </c>
-      <c r="S74">
-        <v>0</v>
-      </c>
-      <c r="T74">
+      <c r="V74">
+        <v>0</v>
+      </c>
+      <c r="W74">
         <v>12791</v>
       </c>
     </row>
-    <row r="75" spans="1:20">
+    <row r="75" spans="1:23">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -5314,23 +5989,32 @@
       <c r="O75">
         <v>73</v>
       </c>
-      <c r="P75" t="s">
-        <v>92</v>
+      <c r="P75">
+        <v>73</v>
       </c>
       <c r="Q75">
+        <v>73</v>
+      </c>
+      <c r="R75">
+        <v>73</v>
+      </c>
+      <c r="S75" t="s">
+        <v>95</v>
+      </c>
+      <c r="T75">
         <v>13268</v>
       </c>
-      <c r="R75">
+      <c r="U75">
         <v>241</v>
       </c>
-      <c r="S75">
-        <v>0</v>
-      </c>
-      <c r="T75">
+      <c r="V75">
+        <v>0</v>
+      </c>
+      <c r="W75">
         <v>13027</v>
       </c>
     </row>
-    <row r="76" spans="1:20">
+    <row r="76" spans="1:23">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -5376,23 +6060,32 @@
       <c r="O76">
         <v>74</v>
       </c>
-      <c r="P76" t="s">
-        <v>93</v>
+      <c r="P76">
+        <v>74</v>
       </c>
       <c r="Q76">
+        <v>74</v>
+      </c>
+      <c r="R76">
+        <v>74</v>
+      </c>
+      <c r="S76" t="s">
+        <v>96</v>
+      </c>
+      <c r="T76">
         <v>13603</v>
       </c>
-      <c r="R76">
+      <c r="U76">
         <v>247</v>
       </c>
-      <c r="S76">
-        <v>0</v>
-      </c>
-      <c r="T76">
+      <c r="V76">
+        <v>0</v>
+      </c>
+      <c r="W76">
         <v>13356</v>
       </c>
     </row>
-    <row r="77" spans="1:20">
+    <row r="77" spans="1:23">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -5438,23 +6131,32 @@
       <c r="O77">
         <v>75</v>
       </c>
-      <c r="P77" t="s">
-        <v>94</v>
+      <c r="P77">
+        <v>75</v>
       </c>
       <c r="Q77">
+        <v>75</v>
+      </c>
+      <c r="R77">
+        <v>75</v>
+      </c>
+      <c r="S77" t="s">
+        <v>97</v>
+      </c>
+      <c r="T77">
         <v>13940</v>
       </c>
-      <c r="R77">
+      <c r="U77">
         <v>253</v>
       </c>
-      <c r="S77">
-        <v>0</v>
-      </c>
-      <c r="T77">
+      <c r="V77">
+        <v>0</v>
+      </c>
+      <c r="W77">
         <v>13687</v>
       </c>
     </row>
-    <row r="78" spans="1:20">
+    <row r="78" spans="1:23">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -5500,23 +6202,32 @@
       <c r="O78">
         <v>76</v>
       </c>
-      <c r="P78" t="s">
-        <v>95</v>
+      <c r="P78">
+        <v>76</v>
       </c>
       <c r="Q78">
+        <v>76</v>
+      </c>
+      <c r="R78">
+        <v>76</v>
+      </c>
+      <c r="S78" t="s">
+        <v>98</v>
+      </c>
+      <c r="T78">
         <v>14423</v>
       </c>
-      <c r="R78">
+      <c r="U78">
         <v>259</v>
       </c>
-      <c r="S78">
-        <v>0</v>
-      </c>
-      <c r="T78">
+      <c r="V78">
+        <v>0</v>
+      </c>
+      <c r="W78">
         <v>14164</v>
       </c>
     </row>
-    <row r="79" spans="1:20">
+    <row r="79" spans="1:23">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -5562,23 +6273,32 @@
       <c r="O79">
         <v>77</v>
       </c>
-      <c r="P79" t="s">
-        <v>96</v>
+      <c r="P79">
+        <v>77</v>
       </c>
       <c r="Q79">
+        <v>77</v>
+      </c>
+      <c r="R79">
+        <v>77</v>
+      </c>
+      <c r="S79" t="s">
+        <v>99</v>
+      </c>
+      <c r="T79">
         <v>14586</v>
       </c>
-      <c r="R79">
+      <c r="U79">
         <v>261</v>
       </c>
-      <c r="S79">
-        <v>0</v>
-      </c>
-      <c r="T79">
+      <c r="V79">
+        <v>0</v>
+      </c>
+      <c r="W79">
         <v>14325</v>
       </c>
     </row>
-    <row r="80" spans="1:20">
+    <row r="80" spans="1:23">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -5624,23 +6344,32 @@
       <c r="O80">
         <v>78</v>
       </c>
-      <c r="P80" t="s">
-        <v>97</v>
+      <c r="P80">
+        <v>78</v>
       </c>
       <c r="Q80">
+        <v>78</v>
+      </c>
+      <c r="R80">
+        <v>78</v>
+      </c>
+      <c r="S80" t="s">
+        <v>100</v>
+      </c>
+      <c r="T80">
         <v>14918</v>
       </c>
-      <c r="R80">
+      <c r="U80">
         <v>262</v>
       </c>
-      <c r="S80">
-        <v>0</v>
-      </c>
-      <c r="T80">
+      <c r="V80">
+        <v>0</v>
+      </c>
+      <c r="W80">
         <v>14656</v>
       </c>
     </row>
-    <row r="81" spans="1:20">
+    <row r="81" spans="1:23">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -5686,23 +6415,32 @@
       <c r="O81">
         <v>79</v>
       </c>
-      <c r="P81" t="s">
-        <v>98</v>
+      <c r="P81">
+        <v>79</v>
       </c>
       <c r="Q81">
+        <v>79</v>
+      </c>
+      <c r="R81">
+        <v>79</v>
+      </c>
+      <c r="S81" t="s">
+        <v>101</v>
+      </c>
+      <c r="T81">
         <v>15238</v>
       </c>
-      <c r="R81">
+      <c r="U81">
         <v>262</v>
       </c>
-      <c r="S81">
-        <v>0</v>
-      </c>
-      <c r="T81">
+      <c r="V81">
+        <v>0</v>
+      </c>
+      <c r="W81">
         <v>14976</v>
       </c>
     </row>
-    <row r="82" spans="1:20">
+    <row r="82" spans="1:23">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -5748,23 +6486,32 @@
       <c r="O82">
         <v>80</v>
       </c>
-      <c r="P82" t="s">
-        <v>99</v>
+      <c r="P82">
+        <v>80</v>
       </c>
       <c r="Q82">
+        <v>80</v>
+      </c>
+      <c r="R82">
+        <v>80</v>
+      </c>
+      <c r="S82" t="s">
+        <v>102</v>
+      </c>
+      <c r="T82">
         <v>15552</v>
       </c>
-      <c r="R82">
+      <c r="U82">
         <v>267</v>
       </c>
-      <c r="S82">
-        <v>0</v>
-      </c>
-      <c r="T82">
+      <c r="V82">
+        <v>0</v>
+      </c>
+      <c r="W82">
         <v>15285</v>
       </c>
     </row>
-    <row r="83" spans="1:20">
+    <row r="83" spans="1:23">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -5810,39 +6557,57 @@
       <c r="O83">
         <v>81</v>
       </c>
-      <c r="P83" t="s">
-        <v>100</v>
+      <c r="P83">
+        <v>81</v>
       </c>
       <c r="Q83">
+        <v>81</v>
+      </c>
+      <c r="R83">
+        <v>81</v>
+      </c>
+      <c r="S83" t="s">
+        <v>103</v>
+      </c>
+      <c r="T83">
         <v>15864</v>
       </c>
-      <c r="R83">
+      <c r="U83">
         <v>267</v>
       </c>
-      <c r="S83">
-        <v>0</v>
-      </c>
-      <c r="T83">
+      <c r="V83">
+        <v>0</v>
+      </c>
+      <c r="W83">
         <v>15597</v>
       </c>
     </row>
-    <row r="84" spans="1:20">
+    <row r="84" spans="1:23">
       <c r="A84" s="1">
         <v>82</v>
       </c>
-      <c r="P84" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q84">
+      <c r="B84">
+        <v>82</v>
+      </c>
+      <c r="C84">
+        <v>82</v>
+      </c>
+      <c r="D84">
+        <v>82</v>
+      </c>
+      <c r="S84" t="s">
+        <v>104</v>
+      </c>
+      <c r="T84">
         <v>16188</v>
       </c>
-      <c r="R84">
+      <c r="U84">
         <v>271</v>
       </c>
-      <c r="S84">
-        <v>0</v>
-      </c>
-      <c r="T84">
+      <c r="V84">
+        <v>0</v>
+      </c>
+      <c r="W84">
         <v>15917</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Travis and Westchester Counties
</commit_message>
<xml_diff>
--- a/Harris_Data.xlsx
+++ b/Harris_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -77,6 +77,21 @@
   </si>
   <si>
     <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
   </si>
   <si>
     <t>Date</t>
@@ -701,13 +716,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA85"/>
+  <dimension ref="A1:AF85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:32">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,8 +801,23 @@
       <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:32">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -854,23 +884,38 @@
       <c r="V2">
         <v>0</v>
       </c>
-      <c r="W2" t="s">
-        <v>26</v>
+      <c r="W2">
+        <v>0</v>
       </c>
       <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC2">
         <v>74</v>
       </c>
-      <c r="Y2">
+      <c r="AD2">
         <v>1</v>
       </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:32">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -937,23 +982,38 @@
       <c r="V3">
         <v>1</v>
       </c>
-      <c r="W3" t="s">
-        <v>27</v>
+      <c r="W3">
+        <v>1</v>
       </c>
       <c r="X3">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="Y3">
         <v>1</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC3">
+        <v>78</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:32">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1020,23 +1080,38 @@
       <c r="V4">
         <v>2</v>
       </c>
-      <c r="W4" t="s">
-        <v>28</v>
+      <c r="W4">
+        <v>2</v>
       </c>
       <c r="X4">
+        <v>2</v>
+      </c>
+      <c r="Y4">
+        <v>2</v>
+      </c>
+      <c r="Z4">
+        <v>2</v>
+      </c>
+      <c r="AA4">
+        <v>2</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC4">
         <v>134</v>
       </c>
-      <c r="Y4">
+      <c r="AD4">
         <v>1</v>
       </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:32">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1103,23 +1178,38 @@
       <c r="V5">
         <v>3</v>
       </c>
-      <c r="W5" t="s">
-        <v>29</v>
+      <c r="W5">
+        <v>3</v>
       </c>
       <c r="X5">
+        <v>3</v>
+      </c>
+      <c r="Y5">
+        <v>3</v>
+      </c>
+      <c r="Z5">
+        <v>3</v>
+      </c>
+      <c r="AA5">
+        <v>3</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC5">
         <v>185</v>
       </c>
-      <c r="Y5">
+      <c r="AD5">
         <v>1</v>
       </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:32">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1186,23 +1276,38 @@
       <c r="V6">
         <v>4</v>
       </c>
-      <c r="W6" t="s">
-        <v>30</v>
+      <c r="W6">
+        <v>4</v>
       </c>
       <c r="X6">
+        <v>4</v>
+      </c>
+      <c r="Y6">
+        <v>4</v>
+      </c>
+      <c r="Z6">
+        <v>4</v>
+      </c>
+      <c r="AA6">
+        <v>4</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC6">
         <v>203</v>
       </c>
-      <c r="Y6">
+      <c r="AD6">
         <v>2</v>
       </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:32">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1269,23 +1374,38 @@
       <c r="V7">
         <v>5</v>
       </c>
-      <c r="W7" t="s">
-        <v>31</v>
+      <c r="W7">
+        <v>5</v>
       </c>
       <c r="X7">
+        <v>5</v>
+      </c>
+      <c r="Y7">
+        <v>5</v>
+      </c>
+      <c r="Z7">
+        <v>5</v>
+      </c>
+      <c r="AA7">
+        <v>5</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC7">
         <v>229</v>
       </c>
-      <c r="Y7">
+      <c r="AD7">
         <v>2</v>
       </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:32">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1352,23 +1472,38 @@
       <c r="V8">
         <v>6</v>
       </c>
-      <c r="W8" t="s">
-        <v>32</v>
+      <c r="W8">
+        <v>6</v>
       </c>
       <c r="X8">
+        <v>6</v>
+      </c>
+      <c r="Y8">
+        <v>6</v>
+      </c>
+      <c r="Z8">
+        <v>6</v>
+      </c>
+      <c r="AA8">
+        <v>6</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC8">
         <v>445</v>
       </c>
-      <c r="Y8">
+      <c r="AD8">
         <v>2</v>
       </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:32">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1435,23 +1570,38 @@
       <c r="V9">
         <v>7</v>
       </c>
-      <c r="W9" t="s">
-        <v>33</v>
+      <c r="W9">
+        <v>7</v>
       </c>
       <c r="X9">
+        <v>7</v>
+      </c>
+      <c r="Y9">
+        <v>7</v>
+      </c>
+      <c r="Z9">
+        <v>7</v>
+      </c>
+      <c r="AA9">
+        <v>7</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC9">
         <v>526</v>
       </c>
-      <c r="Y9">
+      <c r="AD9">
         <v>3</v>
       </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:32">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1518,23 +1668,38 @@
       <c r="V10">
         <v>8</v>
       </c>
-      <c r="W10" t="s">
-        <v>34</v>
+      <c r="W10">
+        <v>8</v>
       </c>
       <c r="X10">
+        <v>8</v>
+      </c>
+      <c r="Y10">
+        <v>8</v>
+      </c>
+      <c r="Z10">
+        <v>8</v>
+      </c>
+      <c r="AA10">
+        <v>8</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC10">
         <v>563</v>
       </c>
-      <c r="Y10">
+      <c r="AD10">
         <v>5</v>
       </c>
-      <c r="Z10">
-        <v>0</v>
-      </c>
-      <c r="AA10">
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:32">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1601,23 +1766,38 @@
       <c r="V11">
         <v>9</v>
       </c>
-      <c r="W11" t="s">
-        <v>35</v>
+      <c r="W11">
+        <v>9</v>
       </c>
       <c r="X11">
+        <v>9</v>
+      </c>
+      <c r="Y11">
+        <v>9</v>
+      </c>
+      <c r="Z11">
+        <v>9</v>
+      </c>
+      <c r="AA11">
+        <v>9</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC11">
         <v>680</v>
       </c>
-      <c r="Y11">
+      <c r="AD11">
         <v>6</v>
       </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:32">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1684,23 +1864,38 @@
       <c r="V12">
         <v>10</v>
       </c>
-      <c r="W12" t="s">
-        <v>36</v>
+      <c r="W12">
+        <v>10</v>
       </c>
       <c r="X12">
+        <v>10</v>
+      </c>
+      <c r="Y12">
+        <v>10</v>
+      </c>
+      <c r="Z12">
+        <v>10</v>
+      </c>
+      <c r="AA12">
+        <v>10</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC12">
         <v>847</v>
       </c>
-      <c r="Y12">
+      <c r="AD12">
         <v>6</v>
       </c>
-      <c r="Z12">
-        <v>0</v>
-      </c>
-      <c r="AA12">
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:32">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1767,23 +1962,38 @@
       <c r="V13">
         <v>11</v>
       </c>
-      <c r="W13" t="s">
-        <v>37</v>
+      <c r="W13">
+        <v>11</v>
       </c>
       <c r="X13">
+        <v>11</v>
+      </c>
+      <c r="Y13">
+        <v>11</v>
+      </c>
+      <c r="Z13">
+        <v>11</v>
+      </c>
+      <c r="AA13">
+        <v>11</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC13">
         <v>955</v>
       </c>
-      <c r="Y13">
+      <c r="AD13">
         <v>6</v>
       </c>
-      <c r="Z13">
-        <v>0</v>
-      </c>
-      <c r="AA13">
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:32">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1850,23 +2060,38 @@
       <c r="V14">
         <v>12</v>
       </c>
-      <c r="W14" t="s">
-        <v>38</v>
+      <c r="W14">
+        <v>12</v>
       </c>
       <c r="X14">
+        <v>12</v>
+      </c>
+      <c r="Y14">
+        <v>12</v>
+      </c>
+      <c r="Z14">
+        <v>12</v>
+      </c>
+      <c r="AA14">
+        <v>12</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC14">
         <v>1106</v>
       </c>
-      <c r="Y14">
+      <c r="AD14">
         <v>13</v>
       </c>
-      <c r="Z14">
-        <v>0</v>
-      </c>
-      <c r="AA14">
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:32">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1933,23 +2158,38 @@
       <c r="V15">
         <v>13</v>
       </c>
-      <c r="W15" t="s">
-        <v>39</v>
+      <c r="W15">
+        <v>13</v>
       </c>
       <c r="X15">
+        <v>13</v>
+      </c>
+      <c r="Y15">
+        <v>13</v>
+      </c>
+      <c r="Z15">
+        <v>13</v>
+      </c>
+      <c r="AA15">
+        <v>13</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC15">
         <v>1284</v>
       </c>
-      <c r="Y15">
+      <c r="AD15">
         <v>17</v>
       </c>
-      <c r="Z15">
-        <v>0</v>
-      </c>
-      <c r="AA15">
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:32">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2016,23 +2256,38 @@
       <c r="V16">
         <v>14</v>
       </c>
-      <c r="W16" t="s">
-        <v>40</v>
+      <c r="W16">
+        <v>14</v>
       </c>
       <c r="X16">
+        <v>14</v>
+      </c>
+      <c r="Y16">
+        <v>14</v>
+      </c>
+      <c r="Z16">
+        <v>14</v>
+      </c>
+      <c r="AA16">
+        <v>14</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC16">
         <v>1395</v>
       </c>
-      <c r="Y16">
+      <c r="AD16">
         <v>20</v>
       </c>
-      <c r="Z16">
-        <v>0</v>
-      </c>
-      <c r="AA16">
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:32">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2099,23 +2354,38 @@
       <c r="V17">
         <v>15</v>
       </c>
-      <c r="W17" t="s">
-        <v>41</v>
+      <c r="W17">
+        <v>15</v>
       </c>
       <c r="X17">
+        <v>15</v>
+      </c>
+      <c r="Y17">
+        <v>15</v>
+      </c>
+      <c r="Z17">
+        <v>15</v>
+      </c>
+      <c r="AA17">
+        <v>15</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC17">
         <v>1809</v>
       </c>
-      <c r="Y17">
+      <c r="AD17">
         <v>22</v>
       </c>
-      <c r="Z17">
-        <v>0</v>
-      </c>
-      <c r="AA17">
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:32">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2182,23 +2452,38 @@
       <c r="V18">
         <v>16</v>
       </c>
-      <c r="W18" t="s">
-        <v>42</v>
+      <c r="W18">
+        <v>16</v>
       </c>
       <c r="X18">
+        <v>16</v>
+      </c>
+      <c r="Y18">
+        <v>16</v>
+      </c>
+      <c r="Z18">
+        <v>16</v>
+      </c>
+      <c r="AA18">
+        <v>16</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC18">
         <v>2146</v>
       </c>
-      <c r="Y18">
+      <c r="AD18">
         <v>23</v>
       </c>
-      <c r="Z18">
-        <v>0</v>
-      </c>
-      <c r="AA18">
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:32">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2265,23 +2550,38 @@
       <c r="V19">
         <v>17</v>
       </c>
-      <c r="W19" t="s">
-        <v>43</v>
+      <c r="W19">
+        <v>17</v>
       </c>
       <c r="X19">
+        <v>17</v>
+      </c>
+      <c r="Y19">
+        <v>17</v>
+      </c>
+      <c r="Z19">
+        <v>17</v>
+      </c>
+      <c r="AA19">
+        <v>17</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC19">
         <v>2341</v>
       </c>
-      <c r="Y19">
+      <c r="AD19">
         <v>31</v>
       </c>
-      <c r="Z19">
-        <v>0</v>
-      </c>
-      <c r="AA19">
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:32">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2348,23 +2648,38 @@
       <c r="V20">
         <v>18</v>
       </c>
-      <c r="W20" t="s">
-        <v>44</v>
+      <c r="W20">
+        <v>18</v>
       </c>
       <c r="X20">
+        <v>18</v>
+      </c>
+      <c r="Y20">
+        <v>18</v>
+      </c>
+      <c r="Z20">
+        <v>18</v>
+      </c>
+      <c r="AA20">
+        <v>18</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC20">
         <v>3047</v>
       </c>
-      <c r="Y20">
+      <c r="AD20">
         <v>34</v>
       </c>
-      <c r="Z20">
-        <v>0</v>
-      </c>
-      <c r="AA20">
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:32">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2431,23 +2746,38 @@
       <c r="V21">
         <v>19</v>
       </c>
-      <c r="W21" t="s">
-        <v>45</v>
+      <c r="W21">
+        <v>19</v>
       </c>
       <c r="X21">
+        <v>19</v>
+      </c>
+      <c r="Y21">
+        <v>19</v>
+      </c>
+      <c r="Z21">
+        <v>19</v>
+      </c>
+      <c r="AA21">
+        <v>19</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC21">
         <v>3261</v>
       </c>
-      <c r="Y21">
+      <c r="AD21">
         <v>40</v>
       </c>
-      <c r="Z21">
-        <v>0</v>
-      </c>
-      <c r="AA21">
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:32">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2514,23 +2844,38 @@
       <c r="V22">
         <v>20</v>
       </c>
-      <c r="W22" t="s">
-        <v>46</v>
+      <c r="W22">
+        <v>20</v>
       </c>
       <c r="X22">
+        <v>20</v>
+      </c>
+      <c r="Y22">
+        <v>20</v>
+      </c>
+      <c r="Z22">
+        <v>20</v>
+      </c>
+      <c r="AA22">
+        <v>20</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC22">
         <v>3561</v>
       </c>
-      <c r="Y22">
+      <c r="AD22">
         <v>41</v>
       </c>
-      <c r="Z22">
-        <v>0</v>
-      </c>
-      <c r="AA22">
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:32">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2597,23 +2942,38 @@
       <c r="V23">
         <v>21</v>
       </c>
-      <c r="W23" t="s">
-        <v>47</v>
+      <c r="W23">
+        <v>21</v>
       </c>
       <c r="X23">
+        <v>21</v>
+      </c>
+      <c r="Y23">
+        <v>21</v>
+      </c>
+      <c r="Z23">
+        <v>21</v>
+      </c>
+      <c r="AA23">
+        <v>21</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC23">
         <v>3629</v>
       </c>
-      <c r="Y23">
+      <c r="AD23">
         <v>44</v>
       </c>
-      <c r="Z23">
-        <v>0</v>
-      </c>
-      <c r="AA23">
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
         <v>3585</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:32">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2680,23 +3040,38 @@
       <c r="V24">
         <v>22</v>
       </c>
-      <c r="W24" t="s">
-        <v>48</v>
+      <c r="W24">
+        <v>22</v>
       </c>
       <c r="X24">
+        <v>22</v>
+      </c>
+      <c r="Y24">
+        <v>22</v>
+      </c>
+      <c r="Z24">
+        <v>22</v>
+      </c>
+      <c r="AA24">
+        <v>22</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC24">
         <v>3744</v>
       </c>
-      <c r="Y24">
+      <c r="AD24">
         <v>46</v>
       </c>
-      <c r="Z24">
-        <v>0</v>
-      </c>
-      <c r="AA24">
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
         <v>3698</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:32">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2763,23 +3138,38 @@
       <c r="V25">
         <v>23</v>
       </c>
-      <c r="W25" t="s">
-        <v>49</v>
+      <c r="W25">
+        <v>23</v>
       </c>
       <c r="X25">
+        <v>23</v>
+      </c>
+      <c r="Y25">
+        <v>23</v>
+      </c>
+      <c r="Z25">
+        <v>23</v>
+      </c>
+      <c r="AA25">
+        <v>23</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC25">
         <v>3907</v>
       </c>
-      <c r="Y25">
+      <c r="AD25">
         <v>52</v>
       </c>
-      <c r="Z25">
-        <v>0</v>
-      </c>
-      <c r="AA25">
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
         <v>3855</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:32">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2846,23 +3236,38 @@
       <c r="V26">
         <v>24</v>
       </c>
-      <c r="W26" t="s">
-        <v>50</v>
+      <c r="W26">
+        <v>24</v>
       </c>
       <c r="X26">
+        <v>24</v>
+      </c>
+      <c r="Y26">
+        <v>24</v>
+      </c>
+      <c r="Z26">
+        <v>24</v>
+      </c>
+      <c r="AA26">
+        <v>24</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC26">
         <v>4097</v>
       </c>
-      <c r="Y26">
+      <c r="AD26">
         <v>58</v>
       </c>
-      <c r="Z26">
-        <v>0</v>
-      </c>
-      <c r="AA26">
+      <c r="AE26">
+        <v>0</v>
+      </c>
+      <c r="AF26">
         <v>4039</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:32">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2929,23 +3334,38 @@
       <c r="V27">
         <v>25</v>
       </c>
-      <c r="W27" t="s">
-        <v>51</v>
+      <c r="W27">
+        <v>25</v>
       </c>
       <c r="X27">
+        <v>25</v>
+      </c>
+      <c r="Y27">
+        <v>25</v>
+      </c>
+      <c r="Z27">
+        <v>25</v>
+      </c>
+      <c r="AA27">
+        <v>25</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC27">
         <v>4306</v>
       </c>
-      <c r="Y27">
+      <c r="AD27">
         <v>63</v>
       </c>
-      <c r="Z27">
-        <v>0</v>
-      </c>
-      <c r="AA27">
+      <c r="AE27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
         <v>4243</v>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:32">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -3012,23 +3432,38 @@
       <c r="V28">
         <v>26</v>
       </c>
-      <c r="W28" t="s">
-        <v>52</v>
+      <c r="W28">
+        <v>26</v>
       </c>
       <c r="X28">
+        <v>26</v>
+      </c>
+      <c r="Y28">
+        <v>26</v>
+      </c>
+      <c r="Z28">
+        <v>26</v>
+      </c>
+      <c r="AA28">
+        <v>26</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC28">
         <v>4460</v>
       </c>
-      <c r="Y28">
+      <c r="AD28">
         <v>67</v>
       </c>
-      <c r="Z28">
-        <v>0</v>
-      </c>
-      <c r="AA28">
+      <c r="AE28">
+        <v>0</v>
+      </c>
+      <c r="AF28">
         <v>4393</v>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:32">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3095,23 +3530,38 @@
       <c r="V29">
         <v>27</v>
       </c>
-      <c r="W29" t="s">
-        <v>53</v>
+      <c r="W29">
+        <v>27</v>
       </c>
       <c r="X29">
+        <v>27</v>
+      </c>
+      <c r="Y29">
+        <v>27</v>
+      </c>
+      <c r="Z29">
+        <v>27</v>
+      </c>
+      <c r="AA29">
+        <v>27</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC29">
         <v>4653</v>
       </c>
-      <c r="Y29">
+      <c r="AD29">
         <v>71</v>
       </c>
-      <c r="Z29">
-        <v>0</v>
-      </c>
-      <c r="AA29">
+      <c r="AE29">
+        <v>0</v>
+      </c>
+      <c r="AF29">
         <v>4582</v>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:32">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3178,23 +3628,38 @@
       <c r="V30">
         <v>28</v>
       </c>
-      <c r="W30" t="s">
-        <v>54</v>
+      <c r="W30">
+        <v>28</v>
       </c>
       <c r="X30">
+        <v>28</v>
+      </c>
+      <c r="Y30">
+        <v>28</v>
+      </c>
+      <c r="Z30">
+        <v>28</v>
+      </c>
+      <c r="AA30">
+        <v>28</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC30">
         <v>4823</v>
       </c>
-      <c r="Y30">
+      <c r="AD30">
         <v>75</v>
       </c>
-      <c r="Z30">
-        <v>0</v>
-      </c>
-      <c r="AA30">
+      <c r="AE30">
+        <v>0</v>
+      </c>
+      <c r="AF30">
         <v>4748</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:32">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3261,23 +3726,38 @@
       <c r="V31">
         <v>29</v>
       </c>
-      <c r="W31" t="s">
-        <v>55</v>
+      <c r="W31">
+        <v>29</v>
       </c>
       <c r="X31">
+        <v>29</v>
+      </c>
+      <c r="Y31">
+        <v>29</v>
+      </c>
+      <c r="Z31">
+        <v>29</v>
+      </c>
+      <c r="AA31">
+        <v>29</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC31">
         <v>4977</v>
       </c>
-      <c r="Y31">
+      <c r="AD31">
         <v>78</v>
       </c>
-      <c r="Z31">
-        <v>0</v>
-      </c>
-      <c r="AA31">
+      <c r="AE31">
+        <v>0</v>
+      </c>
+      <c r="AF31">
         <v>4899</v>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:32">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3344,23 +3824,38 @@
       <c r="V32">
         <v>30</v>
       </c>
-      <c r="W32" t="s">
-        <v>56</v>
+      <c r="W32">
+        <v>30</v>
       </c>
       <c r="X32">
+        <v>30</v>
+      </c>
+      <c r="Y32">
+        <v>30</v>
+      </c>
+      <c r="Z32">
+        <v>30</v>
+      </c>
+      <c r="AA32">
+        <v>30</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC32">
         <v>5143</v>
       </c>
-      <c r="Y32">
+      <c r="AD32">
         <v>79</v>
       </c>
-      <c r="Z32">
-        <v>0</v>
-      </c>
-      <c r="AA32">
+      <c r="AE32">
+        <v>0</v>
+      </c>
+      <c r="AF32">
         <v>5064</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:32">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3427,23 +3922,38 @@
       <c r="V33">
         <v>31</v>
       </c>
-      <c r="W33" t="s">
-        <v>57</v>
+      <c r="W33">
+        <v>31</v>
       </c>
       <c r="X33">
+        <v>31</v>
+      </c>
+      <c r="Y33">
+        <v>31</v>
+      </c>
+      <c r="Z33">
+        <v>31</v>
+      </c>
+      <c r="AA33">
+        <v>31</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC33">
         <v>5211</v>
       </c>
-      <c r="Y33">
+      <c r="AD33">
         <v>80</v>
       </c>
-      <c r="Z33">
-        <v>0</v>
-      </c>
-      <c r="AA33">
+      <c r="AE33">
+        <v>0</v>
+      </c>
+      <c r="AF33">
         <v>5131</v>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:32">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3510,23 +4020,38 @@
       <c r="V34">
         <v>32</v>
       </c>
-      <c r="W34" t="s">
-        <v>58</v>
+      <c r="W34">
+        <v>32</v>
       </c>
       <c r="X34">
+        <v>32</v>
+      </c>
+      <c r="Y34">
+        <v>32</v>
+      </c>
+      <c r="Z34">
+        <v>32</v>
+      </c>
+      <c r="AA34">
+        <v>32</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC34">
         <v>5330</v>
       </c>
-      <c r="Y34">
+      <c r="AD34">
         <v>82</v>
       </c>
-      <c r="Z34">
-        <v>0</v>
-      </c>
-      <c r="AA34">
+      <c r="AE34">
+        <v>0</v>
+      </c>
+      <c r="AF34">
         <v>5248</v>
       </c>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:32">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3593,23 +4118,38 @@
       <c r="V35">
         <v>33</v>
       </c>
-      <c r="W35" t="s">
-        <v>59</v>
+      <c r="W35">
+        <v>33</v>
       </c>
       <c r="X35">
+        <v>33</v>
+      </c>
+      <c r="Y35">
+        <v>33</v>
+      </c>
+      <c r="Z35">
+        <v>33</v>
+      </c>
+      <c r="AA35">
+        <v>33</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC35">
         <v>5482</v>
       </c>
-      <c r="Y35">
+      <c r="AD35">
         <v>84</v>
       </c>
-      <c r="Z35">
-        <v>0</v>
-      </c>
-      <c r="AA35">
+      <c r="AE35">
+        <v>0</v>
+      </c>
+      <c r="AF35">
         <v>5398</v>
       </c>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:32">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3676,23 +4216,38 @@
       <c r="V36">
         <v>34</v>
       </c>
-      <c r="W36" t="s">
-        <v>60</v>
+      <c r="W36">
+        <v>34</v>
       </c>
       <c r="X36">
+        <v>34</v>
+      </c>
+      <c r="Y36">
+        <v>34</v>
+      </c>
+      <c r="Z36">
+        <v>34</v>
+      </c>
+      <c r="AA36">
+        <v>34</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC36">
         <v>5482</v>
       </c>
-      <c r="Y36">
+      <c r="AD36">
         <v>84</v>
       </c>
-      <c r="Z36">
-        <v>0</v>
-      </c>
-      <c r="AA36">
+      <c r="AE36">
+        <v>0</v>
+      </c>
+      <c r="AF36">
         <v>5398</v>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:32">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3759,23 +4314,38 @@
       <c r="V37">
         <v>35</v>
       </c>
-      <c r="W37" t="s">
-        <v>61</v>
+      <c r="W37">
+        <v>35</v>
       </c>
       <c r="X37">
+        <v>35</v>
+      </c>
+      <c r="Y37">
+        <v>35</v>
+      </c>
+      <c r="Z37">
+        <v>35</v>
+      </c>
+      <c r="AA37">
+        <v>35</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC37">
         <v>5628</v>
       </c>
-      <c r="Y37">
+      <c r="AD37">
         <v>84</v>
       </c>
-      <c r="Z37">
-        <v>0</v>
-      </c>
-      <c r="AA37">
+      <c r="AE37">
+        <v>0</v>
+      </c>
+      <c r="AF37">
         <v>5544</v>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:32">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3842,23 +4412,38 @@
       <c r="V38">
         <v>36</v>
       </c>
-      <c r="W38" t="s">
-        <v>62</v>
+      <c r="W38">
+        <v>36</v>
       </c>
       <c r="X38">
+        <v>36</v>
+      </c>
+      <c r="Y38">
+        <v>36</v>
+      </c>
+      <c r="Z38">
+        <v>36</v>
+      </c>
+      <c r="AA38">
+        <v>36</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC38">
         <v>5628</v>
       </c>
-      <c r="Y38">
+      <c r="AD38">
         <v>84</v>
       </c>
-      <c r="Z38">
-        <v>0</v>
-      </c>
-      <c r="AA38">
+      <c r="AE38">
+        <v>0</v>
+      </c>
+      <c r="AF38">
         <v>5544</v>
       </c>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:32">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3925,23 +4510,38 @@
       <c r="V39">
         <v>37</v>
       </c>
-      <c r="W39" t="s">
-        <v>63</v>
+      <c r="W39">
+        <v>37</v>
       </c>
       <c r="X39">
+        <v>37</v>
+      </c>
+      <c r="Y39">
+        <v>37</v>
+      </c>
+      <c r="Z39">
+        <v>37</v>
+      </c>
+      <c r="AA39">
+        <v>37</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC39">
         <v>5827</v>
       </c>
-      <c r="Y39">
+      <c r="AD39">
         <v>98</v>
       </c>
-      <c r="Z39">
-        <v>0</v>
-      </c>
-      <c r="AA39">
+      <c r="AE39">
+        <v>0</v>
+      </c>
+      <c r="AF39">
         <v>5729</v>
       </c>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:32">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -4008,23 +4608,38 @@
       <c r="V40">
         <v>38</v>
       </c>
-      <c r="W40" t="s">
-        <v>64</v>
+      <c r="W40">
+        <v>38</v>
       </c>
       <c r="X40">
+        <v>38</v>
+      </c>
+      <c r="Y40">
+        <v>38</v>
+      </c>
+      <c r="Z40">
+        <v>38</v>
+      </c>
+      <c r="AA40">
+        <v>38</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC40">
         <v>6161</v>
       </c>
-      <c r="Y40">
+      <c r="AD40">
         <v>109</v>
       </c>
-      <c r="Z40">
-        <v>0</v>
-      </c>
-      <c r="AA40">
+      <c r="AE40">
+        <v>0</v>
+      </c>
+      <c r="AF40">
         <v>6052</v>
       </c>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:32">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -4091,23 +4706,38 @@
       <c r="V41">
         <v>39</v>
       </c>
-      <c r="W41" t="s">
-        <v>65</v>
+      <c r="W41">
+        <v>39</v>
       </c>
       <c r="X41">
+        <v>39</v>
+      </c>
+      <c r="Y41">
+        <v>39</v>
+      </c>
+      <c r="Z41">
+        <v>39</v>
+      </c>
+      <c r="AA41">
+        <v>39</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC41">
         <v>6356</v>
       </c>
-      <c r="Y41">
+      <c r="AD41">
         <v>114</v>
       </c>
-      <c r="Z41">
-        <v>0</v>
-      </c>
-      <c r="AA41">
+      <c r="AE41">
+        <v>0</v>
+      </c>
+      <c r="AF41">
         <v>6242</v>
       </c>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:32">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -4174,23 +4804,38 @@
       <c r="V42">
         <v>40</v>
       </c>
-      <c r="W42" t="s">
-        <v>66</v>
+      <c r="W42">
+        <v>40</v>
       </c>
       <c r="X42">
+        <v>40</v>
+      </c>
+      <c r="Y42">
+        <v>40</v>
+      </c>
+      <c r="Z42">
+        <v>40</v>
+      </c>
+      <c r="AA42">
+        <v>40</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC42">
         <v>6551</v>
       </c>
-      <c r="Y42">
+      <c r="AD42">
         <v>122</v>
       </c>
-      <c r="Z42">
-        <v>0</v>
-      </c>
-      <c r="AA42">
+      <c r="AE42">
+        <v>0</v>
+      </c>
+      <c r="AF42">
         <v>6429</v>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:32">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -4257,23 +4902,38 @@
       <c r="V43">
         <v>41</v>
       </c>
-      <c r="W43" t="s">
-        <v>67</v>
+      <c r="W43">
+        <v>41</v>
       </c>
       <c r="X43">
+        <v>41</v>
+      </c>
+      <c r="Y43">
+        <v>41</v>
+      </c>
+      <c r="Z43">
+        <v>41</v>
+      </c>
+      <c r="AA43">
+        <v>41</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC43">
         <v>6708</v>
       </c>
-      <c r="Y43">
+      <c r="AD43">
         <v>129</v>
       </c>
-      <c r="Z43">
-        <v>0</v>
-      </c>
-      <c r="AA43">
+      <c r="AE43">
+        <v>0</v>
+      </c>
+      <c r="AF43">
         <v>6579</v>
       </c>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:32">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -4340,23 +5000,38 @@
       <c r="V44">
         <v>42</v>
       </c>
-      <c r="W44" t="s">
-        <v>68</v>
+      <c r="W44">
+        <v>42</v>
       </c>
       <c r="X44">
+        <v>42</v>
+      </c>
+      <c r="Y44">
+        <v>42</v>
+      </c>
+      <c r="Z44">
+        <v>42</v>
+      </c>
+      <c r="AA44">
+        <v>42</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC44">
         <v>6838</v>
       </c>
-      <c r="Y44">
+      <c r="AD44">
         <v>133</v>
       </c>
-      <c r="Z44">
-        <v>0</v>
-      </c>
-      <c r="AA44">
+      <c r="AE44">
+        <v>0</v>
+      </c>
+      <c r="AF44">
         <v>6705</v>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:32">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4423,23 +5098,38 @@
       <c r="V45">
         <v>43</v>
       </c>
-      <c r="W45" t="s">
-        <v>69</v>
+      <c r="W45">
+        <v>43</v>
       </c>
       <c r="X45">
+        <v>43</v>
+      </c>
+      <c r="Y45">
+        <v>43</v>
+      </c>
+      <c r="Z45">
+        <v>43</v>
+      </c>
+      <c r="AA45">
+        <v>43</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC45">
         <v>6967</v>
       </c>
-      <c r="Y45">
+      <c r="AD45">
         <v>140</v>
       </c>
-      <c r="Z45">
-        <v>0</v>
-      </c>
-      <c r="AA45">
+      <c r="AE45">
+        <v>0</v>
+      </c>
+      <c r="AF45">
         <v>6827</v>
       </c>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:32">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4506,23 +5196,38 @@
       <c r="V46">
         <v>44</v>
       </c>
-      <c r="W46" t="s">
-        <v>70</v>
+      <c r="W46">
+        <v>44</v>
       </c>
       <c r="X46">
+        <v>44</v>
+      </c>
+      <c r="Y46">
+        <v>44</v>
+      </c>
+      <c r="Z46">
+        <v>44</v>
+      </c>
+      <c r="AA46">
+        <v>44</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC46">
         <v>7128</v>
       </c>
-      <c r="Y46">
+      <c r="AD46">
         <v>144</v>
       </c>
-      <c r="Z46">
-        <v>0</v>
-      </c>
-      <c r="AA46">
+      <c r="AE46">
+        <v>0</v>
+      </c>
+      <c r="AF46">
         <v>6984</v>
       </c>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:32">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4589,23 +5294,38 @@
       <c r="V47">
         <v>45</v>
       </c>
-      <c r="W47" t="s">
-        <v>71</v>
+      <c r="W47">
+        <v>45</v>
       </c>
       <c r="X47">
+        <v>45</v>
+      </c>
+      <c r="Y47">
+        <v>45</v>
+      </c>
+      <c r="Z47">
+        <v>45</v>
+      </c>
+      <c r="AA47">
+        <v>45</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC47">
         <v>7244</v>
       </c>
-      <c r="Y47">
+      <c r="AD47">
         <v>150</v>
       </c>
-      <c r="Z47">
-        <v>0</v>
-      </c>
-      <c r="AA47">
+      <c r="AE47">
+        <v>0</v>
+      </c>
+      <c r="AF47">
         <v>7094</v>
       </c>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:32">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4672,23 +5392,38 @@
       <c r="V48">
         <v>46</v>
       </c>
-      <c r="W48" t="s">
-        <v>72</v>
+      <c r="W48">
+        <v>46</v>
       </c>
       <c r="X48">
+        <v>46</v>
+      </c>
+      <c r="Y48">
+        <v>46</v>
+      </c>
+      <c r="Z48">
+        <v>46</v>
+      </c>
+      <c r="AA48">
+        <v>46</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC48">
         <v>7377</v>
       </c>
-      <c r="Y48">
+      <c r="AD48">
         <v>154</v>
       </c>
-      <c r="Z48">
-        <v>0</v>
-      </c>
-      <c r="AA48">
+      <c r="AE48">
+        <v>0</v>
+      </c>
+      <c r="AF48">
         <v>7223</v>
       </c>
     </row>
-    <row r="49" spans="1:27">
+    <row r="49" spans="1:32">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4755,23 +5490,38 @@
       <c r="V49">
         <v>47</v>
       </c>
-      <c r="W49" t="s">
-        <v>73</v>
+      <c r="W49">
+        <v>47</v>
       </c>
       <c r="X49">
+        <v>47</v>
+      </c>
+      <c r="Y49">
+        <v>47</v>
+      </c>
+      <c r="Z49">
+        <v>47</v>
+      </c>
+      <c r="AA49">
+        <v>47</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC49">
         <v>7594</v>
       </c>
-      <c r="Y49">
+      <c r="AD49">
         <v>160</v>
       </c>
-      <c r="Z49">
-        <v>0</v>
-      </c>
-      <c r="AA49">
+      <c r="AE49">
+        <v>0</v>
+      </c>
+      <c r="AF49">
         <v>7434</v>
       </c>
     </row>
-    <row r="50" spans="1:27">
+    <row r="50" spans="1:32">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4838,23 +5588,38 @@
       <c r="V50">
         <v>48</v>
       </c>
-      <c r="W50" t="s">
-        <v>74</v>
+      <c r="W50">
+        <v>48</v>
       </c>
       <c r="X50">
+        <v>48</v>
+      </c>
+      <c r="Y50">
+        <v>48</v>
+      </c>
+      <c r="Z50">
+        <v>48</v>
+      </c>
+      <c r="AA50">
+        <v>48</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC50">
         <v>7803</v>
       </c>
-      <c r="Y50">
+      <c r="AD50">
         <v>168</v>
       </c>
-      <c r="Z50">
-        <v>0</v>
-      </c>
-      <c r="AA50">
+      <c r="AE50">
+        <v>0</v>
+      </c>
+      <c r="AF50">
         <v>7635</v>
       </c>
     </row>
-    <row r="51" spans="1:27">
+    <row r="51" spans="1:32">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4921,23 +5686,38 @@
       <c r="V51">
         <v>49</v>
       </c>
-      <c r="W51" t="s">
-        <v>75</v>
+      <c r="W51">
+        <v>49</v>
       </c>
       <c r="X51">
+        <v>49</v>
+      </c>
+      <c r="Y51">
+        <v>49</v>
+      </c>
+      <c r="Z51">
+        <v>49</v>
+      </c>
+      <c r="AA51">
+        <v>49</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC51">
         <v>7878</v>
       </c>
-      <c r="Y51">
+      <c r="AD51">
         <v>172</v>
       </c>
-      <c r="Z51">
-        <v>0</v>
-      </c>
-      <c r="AA51">
+      <c r="AE51">
+        <v>0</v>
+      </c>
+      <c r="AF51">
         <v>7706</v>
       </c>
     </row>
-    <row r="52" spans="1:27">
+    <row r="52" spans="1:32">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -5004,23 +5784,38 @@
       <c r="V52">
         <v>50</v>
       </c>
-      <c r="W52" t="s">
-        <v>76</v>
+      <c r="W52">
+        <v>50</v>
       </c>
       <c r="X52">
+        <v>50</v>
+      </c>
+      <c r="Y52">
+        <v>50</v>
+      </c>
+      <c r="Z52">
+        <v>50</v>
+      </c>
+      <c r="AA52">
+        <v>50</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC52">
         <v>8176</v>
       </c>
-      <c r="Y52">
+      <c r="AD52">
         <v>179</v>
       </c>
-      <c r="Z52">
-        <v>0</v>
-      </c>
-      <c r="AA52">
+      <c r="AE52">
+        <v>0</v>
+      </c>
+      <c r="AF52">
         <v>7997</v>
       </c>
     </row>
-    <row r="53" spans="1:27">
+    <row r="53" spans="1:32">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -5087,23 +5882,38 @@
       <c r="V53">
         <v>51</v>
       </c>
-      <c r="W53" t="s">
-        <v>77</v>
+      <c r="W53">
+        <v>51</v>
       </c>
       <c r="X53">
+        <v>51</v>
+      </c>
+      <c r="Y53">
+        <v>51</v>
+      </c>
+      <c r="Z53">
+        <v>51</v>
+      </c>
+      <c r="AA53">
+        <v>51</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC53">
         <v>8416</v>
       </c>
-      <c r="Y53">
+      <c r="AD53">
         <v>183</v>
       </c>
-      <c r="Z53">
-        <v>0</v>
-      </c>
-      <c r="AA53">
+      <c r="AE53">
+        <v>0</v>
+      </c>
+      <c r="AF53">
         <v>8233</v>
       </c>
     </row>
-    <row r="54" spans="1:27">
+    <row r="54" spans="1:32">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -5170,23 +5980,38 @@
       <c r="V54">
         <v>52</v>
       </c>
-      <c r="W54" t="s">
-        <v>78</v>
+      <c r="W54">
+        <v>52</v>
       </c>
       <c r="X54">
+        <v>52</v>
+      </c>
+      <c r="Y54">
+        <v>52</v>
+      </c>
+      <c r="Z54">
+        <v>52</v>
+      </c>
+      <c r="AA54">
+        <v>52</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC54">
         <v>8621</v>
       </c>
-      <c r="Y54">
+      <c r="AD54">
         <v>188</v>
       </c>
-      <c r="Z54">
-        <v>0</v>
-      </c>
-      <c r="AA54">
+      <c r="AE54">
+        <v>0</v>
+      </c>
+      <c r="AF54">
         <v>8433</v>
       </c>
     </row>
-    <row r="55" spans="1:27">
+    <row r="55" spans="1:32">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -5253,23 +6078,38 @@
       <c r="V55">
         <v>53</v>
       </c>
-      <c r="W55" t="s">
-        <v>79</v>
+      <c r="W55">
+        <v>53</v>
       </c>
       <c r="X55">
+        <v>53</v>
+      </c>
+      <c r="Y55">
+        <v>53</v>
+      </c>
+      <c r="Z55">
+        <v>53</v>
+      </c>
+      <c r="AA55">
+        <v>53</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC55">
         <v>8817</v>
       </c>
-      <c r="Y55">
+      <c r="AD55">
         <v>193</v>
       </c>
-      <c r="Z55">
-        <v>0</v>
-      </c>
-      <c r="AA55">
+      <c r="AE55">
+        <v>0</v>
+      </c>
+      <c r="AF55">
         <v>8624</v>
       </c>
     </row>
-    <row r="56" spans="1:27">
+    <row r="56" spans="1:32">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -5336,23 +6176,38 @@
       <c r="V56">
         <v>54</v>
       </c>
-      <c r="W56" t="s">
-        <v>80</v>
+      <c r="W56">
+        <v>54</v>
       </c>
       <c r="X56">
+        <v>54</v>
+      </c>
+      <c r="Y56">
+        <v>54</v>
+      </c>
+      <c r="Z56">
+        <v>54</v>
+      </c>
+      <c r="AA56">
+        <v>54</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC56">
         <v>9050</v>
       </c>
-      <c r="Y56">
+      <c r="AD56">
         <v>193</v>
       </c>
-      <c r="Z56">
-        <v>0</v>
-      </c>
-      <c r="AA56">
+      <c r="AE56">
+        <v>0</v>
+      </c>
+      <c r="AF56">
         <v>8857</v>
       </c>
     </row>
-    <row r="57" spans="1:27">
+    <row r="57" spans="1:32">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -5419,23 +6274,38 @@
       <c r="V57">
         <v>55</v>
       </c>
-      <c r="W57" t="s">
-        <v>81</v>
+      <c r="W57">
+        <v>55</v>
       </c>
       <c r="X57">
+        <v>55</v>
+      </c>
+      <c r="Y57">
+        <v>55</v>
+      </c>
+      <c r="Z57">
+        <v>55</v>
+      </c>
+      <c r="AA57">
+        <v>55</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC57">
         <v>9126</v>
       </c>
-      <c r="Y57">
+      <c r="AD57">
         <v>204</v>
       </c>
-      <c r="Z57">
-        <v>0</v>
-      </c>
-      <c r="AA57">
+      <c r="AE57">
+        <v>0</v>
+      </c>
+      <c r="AF57">
         <v>8922</v>
       </c>
     </row>
-    <row r="58" spans="1:27">
+    <row r="58" spans="1:32">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -5502,23 +6372,38 @@
       <c r="V58">
         <v>56</v>
       </c>
-      <c r="W58" t="s">
-        <v>82</v>
+      <c r="W58">
+        <v>56</v>
       </c>
       <c r="X58">
+        <v>56</v>
+      </c>
+      <c r="Y58">
+        <v>56</v>
+      </c>
+      <c r="Z58">
+        <v>56</v>
+      </c>
+      <c r="AA58">
+        <v>56</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC58">
         <v>9465</v>
       </c>
-      <c r="Y58">
+      <c r="AD58">
         <v>204</v>
       </c>
-      <c r="Z58">
-        <v>0</v>
-      </c>
-      <c r="AA58">
+      <c r="AE58">
+        <v>0</v>
+      </c>
+      <c r="AF58">
         <v>9261</v>
       </c>
     </row>
-    <row r="59" spans="1:27">
+    <row r="59" spans="1:32">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -5585,23 +6470,38 @@
       <c r="V59">
         <v>57</v>
       </c>
-      <c r="W59" t="s">
-        <v>83</v>
+      <c r="W59">
+        <v>57</v>
       </c>
       <c r="X59">
+        <v>57</v>
+      </c>
+      <c r="Y59">
+        <v>57</v>
+      </c>
+      <c r="Z59">
+        <v>57</v>
+      </c>
+      <c r="AA59">
+        <v>57</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC59">
         <v>9635</v>
       </c>
-      <c r="Y59">
+      <c r="AD59">
         <v>205</v>
       </c>
-      <c r="Z59">
-        <v>0</v>
-      </c>
-      <c r="AA59">
+      <c r="AE59">
+        <v>0</v>
+      </c>
+      <c r="AF59">
         <v>9430</v>
       </c>
     </row>
-    <row r="60" spans="1:27">
+    <row r="60" spans="1:32">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -5668,23 +6568,38 @@
       <c r="V60">
         <v>58</v>
       </c>
-      <c r="W60" t="s">
-        <v>84</v>
+      <c r="W60">
+        <v>58</v>
       </c>
       <c r="X60">
+        <v>58</v>
+      </c>
+      <c r="Y60">
+        <v>58</v>
+      </c>
+      <c r="Z60">
+        <v>58</v>
+      </c>
+      <c r="AA60">
+        <v>58</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC60">
         <v>9859</v>
       </c>
-      <c r="Y60">
+      <c r="AD60">
         <v>207</v>
       </c>
-      <c r="Z60">
-        <v>0</v>
-      </c>
-      <c r="AA60">
+      <c r="AE60">
+        <v>0</v>
+      </c>
+      <c r="AF60">
         <v>9652</v>
       </c>
     </row>
-    <row r="61" spans="1:27">
+    <row r="61" spans="1:32">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -5751,23 +6666,38 @@
       <c r="V61">
         <v>59</v>
       </c>
-      <c r="W61" t="s">
-        <v>85</v>
+      <c r="W61">
+        <v>59</v>
       </c>
       <c r="X61">
+        <v>59</v>
+      </c>
+      <c r="Y61">
+        <v>59</v>
+      </c>
+      <c r="Z61">
+        <v>59</v>
+      </c>
+      <c r="AA61">
+        <v>59</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC61">
         <v>10095</v>
       </c>
-      <c r="Y61">
+      <c r="AD61">
         <v>210</v>
       </c>
-      <c r="Z61">
-        <v>0</v>
-      </c>
-      <c r="AA61">
+      <c r="AE61">
+        <v>0</v>
+      </c>
+      <c r="AF61">
         <v>9885</v>
       </c>
     </row>
-    <row r="62" spans="1:27">
+    <row r="62" spans="1:32">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -5834,23 +6764,38 @@
       <c r="V62">
         <v>60</v>
       </c>
-      <c r="W62" t="s">
-        <v>86</v>
+      <c r="W62">
+        <v>60</v>
       </c>
       <c r="X62">
+        <v>60</v>
+      </c>
+      <c r="Y62">
+        <v>60</v>
+      </c>
+      <c r="Z62">
+        <v>60</v>
+      </c>
+      <c r="AA62">
+        <v>60</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC62">
         <v>10283</v>
       </c>
-      <c r="Y62">
+      <c r="AD62">
         <v>216</v>
       </c>
-      <c r="Z62">
-        <v>0</v>
-      </c>
-      <c r="AA62">
+      <c r="AE62">
+        <v>0</v>
+      </c>
+      <c r="AF62">
         <v>10067</v>
       </c>
     </row>
-    <row r="63" spans="1:27">
+    <row r="63" spans="1:32">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -5917,23 +6862,38 @@
       <c r="V63">
         <v>61</v>
       </c>
-      <c r="W63" t="s">
-        <v>87</v>
+      <c r="W63">
+        <v>61</v>
       </c>
       <c r="X63">
+        <v>61</v>
+      </c>
+      <c r="Y63">
+        <v>61</v>
+      </c>
+      <c r="Z63">
+        <v>61</v>
+      </c>
+      <c r="AA63">
+        <v>61</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC63">
         <v>10526</v>
       </c>
-      <c r="Y63">
+      <c r="AD63">
         <v>217</v>
       </c>
-      <c r="Z63">
-        <v>0</v>
-      </c>
-      <c r="AA63">
+      <c r="AE63">
+        <v>0</v>
+      </c>
+      <c r="AF63">
         <v>10309</v>
       </c>
     </row>
-    <row r="64" spans="1:27">
+    <row r="64" spans="1:32">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -6000,23 +6960,38 @@
       <c r="V64">
         <v>62</v>
       </c>
-      <c r="W64" t="s">
-        <v>88</v>
+      <c r="W64">
+        <v>62</v>
       </c>
       <c r="X64">
+        <v>62</v>
+      </c>
+      <c r="Y64">
+        <v>62</v>
+      </c>
+      <c r="Z64">
+        <v>62</v>
+      </c>
+      <c r="AA64">
+        <v>62</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC64">
         <v>10770</v>
       </c>
-      <c r="Y64">
+      <c r="AD64">
         <v>219</v>
       </c>
-      <c r="Z64">
-        <v>0</v>
-      </c>
-      <c r="AA64">
+      <c r="AE64">
+        <v>0</v>
+      </c>
+      <c r="AF64">
         <v>10551</v>
       </c>
     </row>
-    <row r="65" spans="1:27">
+    <row r="65" spans="1:32">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -6083,23 +7058,38 @@
       <c r="V65">
         <v>63</v>
       </c>
-      <c r="W65" t="s">
-        <v>89</v>
+      <c r="W65">
+        <v>63</v>
       </c>
       <c r="X65">
+        <v>63</v>
+      </c>
+      <c r="Y65">
+        <v>63</v>
+      </c>
+      <c r="Z65">
+        <v>63</v>
+      </c>
+      <c r="AA65">
+        <v>63</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC65">
         <v>10921</v>
       </c>
-      <c r="Y65">
+      <c r="AD65">
         <v>220</v>
       </c>
-      <c r="Z65">
-        <v>0</v>
-      </c>
-      <c r="AA65">
+      <c r="AE65">
+        <v>0</v>
+      </c>
+      <c r="AF65">
         <v>10701</v>
       </c>
     </row>
-    <row r="66" spans="1:27">
+    <row r="66" spans="1:32">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -6166,23 +7156,38 @@
       <c r="V66">
         <v>64</v>
       </c>
-      <c r="W66" t="s">
-        <v>90</v>
+      <c r="W66">
+        <v>64</v>
       </c>
       <c r="X66">
+        <v>64</v>
+      </c>
+      <c r="Y66">
+        <v>64</v>
+      </c>
+      <c r="Z66">
+        <v>64</v>
+      </c>
+      <c r="AA66">
+        <v>64</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC66">
         <v>10995</v>
       </c>
-      <c r="Y66">
+      <c r="AD66">
         <v>221</v>
       </c>
-      <c r="Z66">
-        <v>0</v>
-      </c>
-      <c r="AA66">
+      <c r="AE66">
+        <v>0</v>
+      </c>
+      <c r="AF66">
         <v>10774</v>
       </c>
     </row>
-    <row r="67" spans="1:27">
+    <row r="67" spans="1:32">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -6249,23 +7254,38 @@
       <c r="V67">
         <v>65</v>
       </c>
-      <c r="W67" t="s">
-        <v>91</v>
+      <c r="W67">
+        <v>65</v>
       </c>
       <c r="X67">
+        <v>65</v>
+      </c>
+      <c r="Y67">
+        <v>65</v>
+      </c>
+      <c r="Z67">
+        <v>65</v>
+      </c>
+      <c r="AA67">
+        <v>65</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC67">
         <v>11281</v>
       </c>
-      <c r="Y67">
+      <c r="AD67">
         <v>221</v>
       </c>
-      <c r="Z67">
-        <v>0</v>
-      </c>
-      <c r="AA67">
+      <c r="AE67">
+        <v>0</v>
+      </c>
+      <c r="AF67">
         <v>11060</v>
       </c>
     </row>
-    <row r="68" spans="1:27">
+    <row r="68" spans="1:32">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -6332,23 +7352,38 @@
       <c r="V68">
         <v>66</v>
       </c>
-      <c r="W68" t="s">
-        <v>92</v>
+      <c r="W68">
+        <v>66</v>
       </c>
       <c r="X68">
+        <v>66</v>
+      </c>
+      <c r="Y68">
+        <v>66</v>
+      </c>
+      <c r="Z68">
+        <v>66</v>
+      </c>
+      <c r="AA68">
+        <v>66</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC68">
         <v>11542</v>
       </c>
-      <c r="Y68">
+      <c r="AD68">
         <v>223</v>
       </c>
-      <c r="Z68">
-        <v>0</v>
-      </c>
-      <c r="AA68">
+      <c r="AE68">
+        <v>0</v>
+      </c>
+      <c r="AF68">
         <v>11319</v>
       </c>
     </row>
-    <row r="69" spans="1:27">
+    <row r="69" spans="1:32">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -6415,23 +7450,38 @@
       <c r="V69">
         <v>67</v>
       </c>
-      <c r="W69" t="s">
-        <v>93</v>
+      <c r="W69">
+        <v>67</v>
       </c>
       <c r="X69">
+        <v>67</v>
+      </c>
+      <c r="Y69">
+        <v>67</v>
+      </c>
+      <c r="Z69">
+        <v>67</v>
+      </c>
+      <c r="AA69">
+        <v>67</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC69">
         <v>11770</v>
       </c>
-      <c r="Y69">
+      <c r="AD69">
         <v>224</v>
       </c>
-      <c r="Z69">
-        <v>0</v>
-      </c>
-      <c r="AA69">
+      <c r="AE69">
+        <v>0</v>
+      </c>
+      <c r="AF69">
         <v>11546</v>
       </c>
     </row>
-    <row r="70" spans="1:27">
+    <row r="70" spans="1:32">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -6498,23 +7548,38 @@
       <c r="V70">
         <v>68</v>
       </c>
-      <c r="W70" t="s">
-        <v>94</v>
+      <c r="W70">
+        <v>68</v>
       </c>
       <c r="X70">
+        <v>68</v>
+      </c>
+      <c r="Y70">
+        <v>68</v>
+      </c>
+      <c r="Z70">
+        <v>68</v>
+      </c>
+      <c r="AA70">
+        <v>68</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC70">
         <v>12009</v>
       </c>
-      <c r="Y70">
+      <c r="AD70">
         <v>228</v>
       </c>
-      <c r="Z70">
-        <v>0</v>
-      </c>
-      <c r="AA70">
+      <c r="AE70">
+        <v>0</v>
+      </c>
+      <c r="AF70">
         <v>11781</v>
       </c>
     </row>
-    <row r="71" spans="1:27">
+    <row r="71" spans="1:32">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -6581,23 +7646,38 @@
       <c r="V71">
         <v>69</v>
       </c>
-      <c r="W71" t="s">
-        <v>95</v>
+      <c r="W71">
+        <v>69</v>
       </c>
       <c r="X71">
+        <v>69</v>
+      </c>
+      <c r="Y71">
+        <v>69</v>
+      </c>
+      <c r="Z71">
+        <v>69</v>
+      </c>
+      <c r="AA71">
+        <v>69</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC71">
         <v>12220</v>
       </c>
-      <c r="Y71">
+      <c r="AD71">
         <v>231</v>
       </c>
-      <c r="Z71">
-        <v>0</v>
-      </c>
-      <c r="AA71">
+      <c r="AE71">
+        <v>0</v>
+      </c>
+      <c r="AF71">
         <v>11989</v>
       </c>
     </row>
-    <row r="72" spans="1:27">
+    <row r="72" spans="1:32">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -6664,23 +7744,38 @@
       <c r="V72">
         <v>70</v>
       </c>
-      <c r="W72" t="s">
-        <v>96</v>
+      <c r="W72">
+        <v>70</v>
       </c>
       <c r="X72">
+        <v>70</v>
+      </c>
+      <c r="Y72">
+        <v>70</v>
+      </c>
+      <c r="Z72">
+        <v>70</v>
+      </c>
+      <c r="AA72">
+        <v>70</v>
+      </c>
+      <c r="AB72" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC72">
         <v>12276</v>
       </c>
-      <c r="Y72">
+      <c r="AD72">
         <v>232</v>
       </c>
-      <c r="Z72">
-        <v>0</v>
-      </c>
-      <c r="AA72">
+      <c r="AE72">
+        <v>0</v>
+      </c>
+      <c r="AF72">
         <v>12044</v>
       </c>
     </row>
-    <row r="73" spans="1:27">
+    <row r="73" spans="1:32">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -6747,23 +7842,38 @@
       <c r="V73">
         <v>71</v>
       </c>
-      <c r="W73" t="s">
-        <v>97</v>
+      <c r="W73">
+        <v>71</v>
       </c>
       <c r="X73">
+        <v>71</v>
+      </c>
+      <c r="Y73">
+        <v>71</v>
+      </c>
+      <c r="Z73">
+        <v>71</v>
+      </c>
+      <c r="AA73">
+        <v>71</v>
+      </c>
+      <c r="AB73" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC73">
         <v>12664</v>
       </c>
-      <c r="Y73">
+      <c r="AD73">
         <v>235</v>
       </c>
-      <c r="Z73">
-        <v>0</v>
-      </c>
-      <c r="AA73">
+      <c r="AE73">
+        <v>0</v>
+      </c>
+      <c r="AF73">
         <v>12429</v>
       </c>
     </row>
-    <row r="74" spans="1:27">
+    <row r="74" spans="1:32">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -6830,23 +7940,38 @@
       <c r="V74">
         <v>72</v>
       </c>
-      <c r="W74" t="s">
-        <v>98</v>
+      <c r="W74">
+        <v>72</v>
       </c>
       <c r="X74">
+        <v>72</v>
+      </c>
+      <c r="Y74">
+        <v>72</v>
+      </c>
+      <c r="Z74">
+        <v>72</v>
+      </c>
+      <c r="AA74">
+        <v>72</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC74">
         <v>13027</v>
       </c>
-      <c r="Y74">
+      <c r="AD74">
         <v>236</v>
       </c>
-      <c r="Z74">
-        <v>0</v>
-      </c>
-      <c r="AA74">
+      <c r="AE74">
+        <v>0</v>
+      </c>
+      <c r="AF74">
         <v>12791</v>
       </c>
     </row>
-    <row r="75" spans="1:27">
+    <row r="75" spans="1:32">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -6913,23 +8038,38 @@
       <c r="V75">
         <v>73</v>
       </c>
-      <c r="W75" t="s">
-        <v>99</v>
+      <c r="W75">
+        <v>73</v>
       </c>
       <c r="X75">
+        <v>73</v>
+      </c>
+      <c r="Y75">
+        <v>73</v>
+      </c>
+      <c r="Z75">
+        <v>73</v>
+      </c>
+      <c r="AA75">
+        <v>73</v>
+      </c>
+      <c r="AB75" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC75">
         <v>13268</v>
       </c>
-      <c r="Y75">
+      <c r="AD75">
         <v>241</v>
       </c>
-      <c r="Z75">
-        <v>0</v>
-      </c>
-      <c r="AA75">
+      <c r="AE75">
+        <v>0</v>
+      </c>
+      <c r="AF75">
         <v>13027</v>
       </c>
     </row>
-    <row r="76" spans="1:27">
+    <row r="76" spans="1:32">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -6996,23 +8136,38 @@
       <c r="V76">
         <v>74</v>
       </c>
-      <c r="W76" t="s">
-        <v>100</v>
+      <c r="W76">
+        <v>74</v>
       </c>
       <c r="X76">
+        <v>74</v>
+      </c>
+      <c r="Y76">
+        <v>74</v>
+      </c>
+      <c r="Z76">
+        <v>74</v>
+      </c>
+      <c r="AA76">
+        <v>74</v>
+      </c>
+      <c r="AB76" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC76">
         <v>13603</v>
       </c>
-      <c r="Y76">
+      <c r="AD76">
         <v>247</v>
       </c>
-      <c r="Z76">
-        <v>0</v>
-      </c>
-      <c r="AA76">
+      <c r="AE76">
+        <v>0</v>
+      </c>
+      <c r="AF76">
         <v>13356</v>
       </c>
     </row>
-    <row r="77" spans="1:27">
+    <row r="77" spans="1:32">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -7079,23 +8234,38 @@
       <c r="V77">
         <v>75</v>
       </c>
-      <c r="W77" t="s">
-        <v>101</v>
+      <c r="W77">
+        <v>75</v>
       </c>
       <c r="X77">
+        <v>75</v>
+      </c>
+      <c r="Y77">
+        <v>75</v>
+      </c>
+      <c r="Z77">
+        <v>75</v>
+      </c>
+      <c r="AA77">
+        <v>75</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC77">
         <v>13940</v>
       </c>
-      <c r="Y77">
+      <c r="AD77">
         <v>253</v>
       </c>
-      <c r="Z77">
-        <v>0</v>
-      </c>
-      <c r="AA77">
+      <c r="AE77">
+        <v>0</v>
+      </c>
+      <c r="AF77">
         <v>13687</v>
       </c>
     </row>
-    <row r="78" spans="1:27">
+    <row r="78" spans="1:32">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -7162,23 +8332,38 @@
       <c r="V78">
         <v>76</v>
       </c>
-      <c r="W78" t="s">
-        <v>102</v>
+      <c r="W78">
+        <v>76</v>
       </c>
       <c r="X78">
+        <v>76</v>
+      </c>
+      <c r="Y78">
+        <v>76</v>
+      </c>
+      <c r="Z78">
+        <v>76</v>
+      </c>
+      <c r="AA78">
+        <v>76</v>
+      </c>
+      <c r="AB78" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC78">
         <v>14423</v>
       </c>
-      <c r="Y78">
+      <c r="AD78">
         <v>259</v>
       </c>
-      <c r="Z78">
-        <v>0</v>
-      </c>
-      <c r="AA78">
+      <c r="AE78">
+        <v>0</v>
+      </c>
+      <c r="AF78">
         <v>14164</v>
       </c>
     </row>
-    <row r="79" spans="1:27">
+    <row r="79" spans="1:32">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -7245,23 +8430,38 @@
       <c r="V79">
         <v>77</v>
       </c>
-      <c r="W79" t="s">
-        <v>103</v>
+      <c r="W79">
+        <v>77</v>
       </c>
       <c r="X79">
+        <v>77</v>
+      </c>
+      <c r="Y79">
+        <v>77</v>
+      </c>
+      <c r="Z79">
+        <v>77</v>
+      </c>
+      <c r="AA79">
+        <v>77</v>
+      </c>
+      <c r="AB79" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC79">
         <v>14586</v>
       </c>
-      <c r="Y79">
+      <c r="AD79">
         <v>261</v>
       </c>
-      <c r="Z79">
-        <v>0</v>
-      </c>
-      <c r="AA79">
+      <c r="AE79">
+        <v>0</v>
+      </c>
+      <c r="AF79">
         <v>14325</v>
       </c>
     </row>
-    <row r="80" spans="1:27">
+    <row r="80" spans="1:32">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -7328,23 +8528,38 @@
       <c r="V80">
         <v>78</v>
       </c>
-      <c r="W80" t="s">
-        <v>104</v>
+      <c r="W80">
+        <v>78</v>
       </c>
       <c r="X80">
+        <v>78</v>
+      </c>
+      <c r="Y80">
+        <v>78</v>
+      </c>
+      <c r="Z80">
+        <v>78</v>
+      </c>
+      <c r="AA80">
+        <v>78</v>
+      </c>
+      <c r="AB80" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC80">
         <v>14918</v>
       </c>
-      <c r="Y80">
+      <c r="AD80">
         <v>262</v>
       </c>
-      <c r="Z80">
-        <v>0</v>
-      </c>
-      <c r="AA80">
+      <c r="AE80">
+        <v>0</v>
+      </c>
+      <c r="AF80">
         <v>14656</v>
       </c>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:32">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -7411,23 +8626,38 @@
       <c r="V81">
         <v>79</v>
       </c>
-      <c r="W81" t="s">
-        <v>105</v>
+      <c r="W81">
+        <v>79</v>
       </c>
       <c r="X81">
+        <v>79</v>
+      </c>
+      <c r="Y81">
+        <v>79</v>
+      </c>
+      <c r="Z81">
+        <v>79</v>
+      </c>
+      <c r="AA81">
+        <v>79</v>
+      </c>
+      <c r="AB81" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC81">
         <v>15238</v>
       </c>
-      <c r="Y81">
+      <c r="AD81">
         <v>262</v>
       </c>
-      <c r="Z81">
-        <v>0</v>
-      </c>
-      <c r="AA81">
+      <c r="AE81">
+        <v>0</v>
+      </c>
+      <c r="AF81">
         <v>14976</v>
       </c>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:32">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -7494,23 +8724,38 @@
       <c r="V82">
         <v>80</v>
       </c>
-      <c r="W82" t="s">
-        <v>106</v>
+      <c r="W82">
+        <v>80</v>
       </c>
       <c r="X82">
+        <v>80</v>
+      </c>
+      <c r="Y82">
+        <v>80</v>
+      </c>
+      <c r="Z82">
+        <v>80</v>
+      </c>
+      <c r="AA82">
+        <v>80</v>
+      </c>
+      <c r="AB82" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC82">
         <v>15552</v>
       </c>
-      <c r="Y82">
+      <c r="AD82">
         <v>267</v>
       </c>
-      <c r="Z82">
-        <v>0</v>
-      </c>
-      <c r="AA82">
+      <c r="AE82">
+        <v>0</v>
+      </c>
+      <c r="AF82">
         <v>15285</v>
       </c>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:32">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -7577,23 +8822,38 @@
       <c r="V83">
         <v>81</v>
       </c>
-      <c r="W83" t="s">
-        <v>107</v>
+      <c r="W83">
+        <v>81</v>
       </c>
       <c r="X83">
+        <v>81</v>
+      </c>
+      <c r="Y83">
+        <v>81</v>
+      </c>
+      <c r="Z83">
+        <v>81</v>
+      </c>
+      <c r="AA83">
+        <v>81</v>
+      </c>
+      <c r="AB83" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC83">
         <v>15864</v>
       </c>
-      <c r="Y83">
+      <c r="AD83">
         <v>267</v>
       </c>
-      <c r="Z83">
-        <v>0</v>
-      </c>
-      <c r="AA83">
+      <c r="AE83">
+        <v>0</v>
+      </c>
+      <c r="AF83">
         <v>15597</v>
       </c>
     </row>
-    <row r="84" spans="1:27">
+    <row r="84" spans="1:32">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -7618,23 +8878,38 @@
       <c r="H84">
         <v>82</v>
       </c>
-      <c r="W84" t="s">
-        <v>108</v>
-      </c>
-      <c r="X84">
+      <c r="I84">
+        <v>82</v>
+      </c>
+      <c r="J84">
+        <v>82</v>
+      </c>
+      <c r="K84">
+        <v>82</v>
+      </c>
+      <c r="L84">
+        <v>82</v>
+      </c>
+      <c r="M84">
+        <v>82</v>
+      </c>
+      <c r="AB84" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC84">
         <v>16188</v>
       </c>
-      <c r="Y84">
+      <c r="AD84">
         <v>271</v>
       </c>
-      <c r="Z84">
-        <v>0</v>
-      </c>
-      <c r="AA84">
+      <c r="AE84">
+        <v>0</v>
+      </c>
+      <c r="AF84">
         <v>15917</v>
       </c>
     </row>
-    <row r="85" spans="1:27">
+    <row r="85" spans="1:32">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -7647,19 +8922,34 @@
       <c r="D85">
         <v>83</v>
       </c>
-      <c r="W85" t="s">
-        <v>109</v>
-      </c>
-      <c r="X85">
+      <c r="E85">
+        <v>83</v>
+      </c>
+      <c r="F85">
+        <v>83</v>
+      </c>
+      <c r="G85">
+        <v>83</v>
+      </c>
+      <c r="H85">
+        <v>83</v>
+      </c>
+      <c r="I85">
+        <v>83</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC85">
         <v>16568</v>
       </c>
-      <c r="Y85">
+      <c r="AD85">
         <v>275</v>
       </c>
-      <c r="Z85">
-        <v>0</v>
-      </c>
-      <c r="AA85">
+      <c r="AE85">
+        <v>0</v>
+      </c>
+      <c r="AF85">
         <v>16293</v>
       </c>
     </row>

</xml_diff>